<commit_message>
implemented changes to the map window and shapefile to focus on the 5 provinces of interest in Indonesia
</commit_message>
<xml_diff>
--- a/Data/Indonesia/Misc/ShapefileAddingIndonesia.xlsx
+++ b/Data/Indonesia/Misc/ShapefileAddingIndonesia.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20364"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20366"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\slomb\OneDrive\Desktop\SD_UI\Data\Indonesia\Misc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{65B4F646-7FF6-4C50-8AFD-5F80061DCE38}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9962179-E5BB-40BA-9D98-F0CD02F40E5F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6045"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6045" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ShapefileAddingIndonesia" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
@@ -259,7 +259,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1094,15 +1094,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31:J35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="27.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11" bestFit="1" customWidth="1"/>
@@ -1148,28 +1149,28 @@
         <v>5</v>
       </c>
       <c r="C2">
-        <v>415</v>
+        <v>0</v>
       </c>
       <c r="D2">
-        <v>91</v>
+        <v>0</v>
       </c>
       <c r="E2">
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="F2">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="G2">
-        <v>-11</v>
+        <v>0</v>
       </c>
       <c r="H2">
-        <v>-28</v>
+        <v>0</v>
       </c>
       <c r="I2">
-        <v>-10</v>
+        <v>0</v>
       </c>
       <c r="J2">
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -1179,29 +1180,29 @@
       <c r="B3" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="1">
-        <v>3407</v>
-      </c>
-      <c r="D3" s="1">
-        <v>2876</v>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
       </c>
       <c r="E3">
-        <v>-34</v>
+        <v>0</v>
       </c>
       <c r="F3">
-        <v>-26</v>
+        <v>0</v>
       </c>
       <c r="G3">
-        <v>-43</v>
+        <v>0</v>
       </c>
       <c r="H3">
-        <v>-69</v>
+        <v>0</v>
       </c>
       <c r="I3">
-        <v>-37</v>
+        <v>0</v>
       </c>
       <c r="J3">
-        <v>15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -1212,28 +1213,28 @@
         <v>9</v>
       </c>
       <c r="C4">
-        <v>193</v>
+        <v>0</v>
       </c>
       <c r="D4">
-        <v>173</v>
+        <v>0</v>
       </c>
       <c r="E4">
-        <v>-13</v>
+        <v>0</v>
       </c>
       <c r="F4">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="G4">
-        <v>-9</v>
+        <v>0</v>
       </c>
       <c r="H4">
-        <v>-36</v>
+        <v>0</v>
       </c>
       <c r="I4">
-        <v>-15</v>
+        <v>0</v>
       </c>
       <c r="J4">
-        <v>9</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -1243,29 +1244,29 @@
       <c r="B5" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="1">
-        <v>1835</v>
-      </c>
-      <c r="D5" s="1">
-        <v>1354</v>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
       </c>
       <c r="E5">
-        <v>-11</v>
+        <v>0</v>
       </c>
       <c r="F5">
-        <v>-6</v>
+        <v>0</v>
       </c>
       <c r="G5">
-        <v>-4</v>
+        <v>0</v>
       </c>
       <c r="H5">
-        <v>-47</v>
+        <v>0</v>
       </c>
       <c r="I5">
-        <v>-23</v>
+        <v>0</v>
       </c>
       <c r="J5">
-        <v>14</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -1276,28 +1277,28 @@
         <v>13</v>
       </c>
       <c r="C6">
-        <v>217</v>
+        <v>0</v>
       </c>
       <c r="D6">
-        <v>118</v>
+        <v>0</v>
       </c>
       <c r="E6">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="F6">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="G6">
-        <v>-3</v>
+        <v>0</v>
       </c>
       <c r="H6">
-        <v>-30</v>
+        <v>0</v>
       </c>
       <c r="I6">
-        <v>-16</v>
+        <v>0</v>
       </c>
       <c r="J6">
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -1339,29 +1340,29 @@
       <c r="B8" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="1">
-        <v>1729</v>
-      </c>
-      <c r="D8" s="1">
-        <v>1182</v>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
       </c>
       <c r="E8">
-        <v>-14</v>
+        <v>0</v>
       </c>
       <c r="F8">
-        <v>-6</v>
+        <v>0</v>
       </c>
       <c r="G8">
-        <v>-16</v>
+        <v>0</v>
       </c>
       <c r="H8">
-        <v>-27</v>
+        <v>0</v>
       </c>
       <c r="I8">
-        <v>-16</v>
+        <v>0</v>
       </c>
       <c r="J8">
-        <v>9</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -1372,28 +1373,28 @@
         <v>19</v>
       </c>
       <c r="C9">
-        <v>207</v>
+        <v>0</v>
       </c>
       <c r="D9">
-        <v>188</v>
+        <v>0</v>
       </c>
       <c r="E9">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="F9">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="G9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H9">
-        <v>-29</v>
+        <v>0</v>
       </c>
       <c r="I9">
-        <v>-11</v>
+        <v>0</v>
       </c>
       <c r="J9">
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -1435,29 +1436,29 @@
       <c r="B11" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="1">
-        <v>1426</v>
+      <c r="C11">
+        <v>0</v>
       </c>
       <c r="D11">
-        <v>903</v>
+        <v>0</v>
       </c>
       <c r="E11">
-        <v>-13</v>
+        <v>0</v>
       </c>
       <c r="F11">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="G11">
-        <v>-10</v>
+        <v>0</v>
       </c>
       <c r="H11">
-        <v>-34</v>
+        <v>0</v>
       </c>
       <c r="I11">
-        <v>-19</v>
+        <v>0</v>
       </c>
       <c r="J11">
-        <v>11</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -1468,28 +1469,28 @@
         <v>25</v>
       </c>
       <c r="C12">
-        <v>145</v>
+        <v>0</v>
       </c>
       <c r="D12">
-        <v>110</v>
+        <v>0</v>
       </c>
       <c r="E12">
-        <v>-7</v>
+        <v>0</v>
       </c>
       <c r="F12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G12">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H12">
-        <v>-19</v>
+        <v>0</v>
       </c>
       <c r="I12">
-        <v>-7</v>
+        <v>0</v>
       </c>
       <c r="J12">
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -1499,29 +1500,29 @@
       <c r="B13" t="s">
         <v>27</v>
       </c>
-      <c r="C13" s="1">
-        <v>1015</v>
+      <c r="C13">
+        <v>0</v>
       </c>
       <c r="D13">
-        <v>544</v>
+        <v>0</v>
       </c>
       <c r="E13">
-        <v>-4</v>
+        <v>0</v>
       </c>
       <c r="F13">
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="G13">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="H13">
         <v>0</v>
       </c>
       <c r="I13">
-        <v>-17</v>
+        <v>0</v>
       </c>
       <c r="J13">
-        <v>13</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -1564,28 +1565,28 @@
         <v>31</v>
       </c>
       <c r="C15">
-        <v>162</v>
+        <v>0</v>
       </c>
       <c r="D15">
-        <v>115</v>
+        <v>0</v>
       </c>
       <c r="E15">
-        <v>-11</v>
+        <v>0</v>
       </c>
       <c r="F15">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G15">
-        <v>-12</v>
+        <v>0</v>
       </c>
       <c r="H15">
-        <v>-27</v>
+        <v>0</v>
       </c>
       <c r="I15">
-        <v>-14</v>
+        <v>0</v>
       </c>
       <c r="J15">
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -1596,28 +1597,28 @@
         <v>33</v>
       </c>
       <c r="C16">
-        <v>255</v>
+        <v>0</v>
       </c>
       <c r="D16">
-        <v>195</v>
+        <v>0</v>
       </c>
       <c r="E16">
-        <v>-3</v>
+        <v>0</v>
       </c>
       <c r="F16">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="G16">
-        <v>-8</v>
+        <v>0</v>
       </c>
       <c r="H16">
-        <v>-29</v>
+        <v>0</v>
       </c>
       <c r="I16">
-        <v>-20</v>
+        <v>0</v>
       </c>
       <c r="J16">
-        <v>9</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
@@ -1627,29 +1628,29 @@
       <c r="B17" t="s">
         <v>35</v>
       </c>
-      <c r="C17" s="1">
-        <v>1093</v>
+      <c r="C17">
+        <v>0</v>
       </c>
       <c r="D17">
-        <v>699</v>
+        <v>0</v>
       </c>
       <c r="E17">
-        <v>-20</v>
+        <v>0</v>
       </c>
       <c r="F17">
-        <v>-11</v>
+        <v>0</v>
       </c>
       <c r="G17">
-        <v>-14</v>
+        <v>0</v>
       </c>
       <c r="H17">
-        <v>-33</v>
+        <v>0</v>
       </c>
       <c r="I17">
-        <v>-20</v>
+        <v>0</v>
       </c>
       <c r="J17">
-        <v>11</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
@@ -1660,28 +1661,28 @@
         <v>37</v>
       </c>
       <c r="C18">
-        <v>283</v>
+        <v>0</v>
       </c>
       <c r="D18">
-        <v>214</v>
+        <v>0</v>
       </c>
       <c r="E18">
-        <v>-12</v>
+        <v>0</v>
       </c>
       <c r="F18">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="G18">
-        <v>-7</v>
+        <v>0</v>
       </c>
       <c r="H18">
-        <v>-29</v>
+        <v>0</v>
       </c>
       <c r="I18">
-        <v>-11</v>
+        <v>0</v>
       </c>
       <c r="J18">
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
@@ -1691,29 +1692,29 @@
       <c r="B19" t="s">
         <v>39</v>
       </c>
-      <c r="C19" s="1">
-        <v>1530</v>
+      <c r="C19">
+        <v>0</v>
       </c>
       <c r="D19">
-        <v>328</v>
+        <v>0</v>
       </c>
       <c r="E19">
-        <v>-21</v>
+        <v>0</v>
       </c>
       <c r="F19">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="G19">
-        <v>-20</v>
+        <v>0</v>
       </c>
       <c r="H19">
-        <v>-9</v>
+        <v>0</v>
       </c>
       <c r="I19">
-        <v>-18</v>
+        <v>0</v>
       </c>
       <c r="J19">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
@@ -1723,29 +1724,29 @@
       <c r="B20" t="s">
         <v>41</v>
       </c>
-      <c r="C20" s="1">
-        <v>2580</v>
-      </c>
-      <c r="D20" s="1">
-        <v>1205</v>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
       </c>
       <c r="E20">
-        <v>-27</v>
+        <v>0</v>
       </c>
       <c r="F20">
-        <v>-8</v>
+        <v>0</v>
       </c>
       <c r="G20">
-        <v>-20</v>
+        <v>0</v>
       </c>
       <c r="H20">
-        <v>-45</v>
+        <v>0</v>
       </c>
       <c r="I20">
-        <v>-22</v>
+        <v>0</v>
       </c>
       <c r="J20">
-        <v>13</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
@@ -1755,29 +1756,29 @@
       <c r="B21" t="s">
         <v>43</v>
       </c>
-      <c r="C21" s="1">
-        <v>3931</v>
-      </c>
-      <c r="D21" s="1">
-        <v>1353</v>
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
       </c>
       <c r="E21">
-        <v>-20</v>
+        <v>0</v>
       </c>
       <c r="F21">
-        <v>-11</v>
+        <v>0</v>
       </c>
       <c r="G21">
-        <v>-16</v>
+        <v>0</v>
       </c>
       <c r="H21">
-        <v>-36</v>
+        <v>0</v>
       </c>
       <c r="I21">
-        <v>-22</v>
+        <v>0</v>
       </c>
       <c r="J21">
-        <v>11</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
@@ -1787,29 +1788,29 @@
       <c r="B22" t="s">
         <v>45</v>
       </c>
-      <c r="C22" s="1">
-        <v>3059</v>
-      </c>
-      <c r="D22" s="1">
-        <v>1375</v>
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
       </c>
       <c r="E22">
-        <v>-20</v>
+        <v>0</v>
       </c>
       <c r="F22">
-        <v>-11</v>
+        <v>0</v>
       </c>
       <c r="G22">
-        <v>-10</v>
+        <v>0</v>
       </c>
       <c r="H22">
-        <v>-31</v>
+        <v>0</v>
       </c>
       <c r="I22">
-        <v>-14</v>
+        <v>0</v>
       </c>
       <c r="J22">
-        <v>9</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
@@ -1820,28 +1821,28 @@
         <v>47</v>
       </c>
       <c r="C23">
-        <v>445</v>
+        <v>0</v>
       </c>
       <c r="D23">
-        <v>308</v>
+        <v>0</v>
       </c>
       <c r="E23">
-        <v>-9</v>
+        <v>0</v>
       </c>
       <c r="F23">
-        <v>-3</v>
+        <v>0</v>
       </c>
       <c r="G23">
-        <v>-5</v>
+        <v>0</v>
       </c>
       <c r="H23">
-        <v>-41</v>
+        <v>0</v>
       </c>
       <c r="I23">
-        <v>-15</v>
+        <v>0</v>
       </c>
       <c r="J23">
-        <v>9</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
@@ -1852,28 +1853,28 @@
         <v>49</v>
       </c>
       <c r="C24">
-        <v>447</v>
+        <v>0</v>
       </c>
       <c r="D24">
-        <v>321</v>
+        <v>0</v>
       </c>
       <c r="E24">
-        <v>-20</v>
+        <v>0</v>
       </c>
       <c r="F24">
-        <v>-12</v>
+        <v>0</v>
       </c>
       <c r="G24">
-        <v>-25</v>
+        <v>0</v>
       </c>
       <c r="H24">
-        <v>-50</v>
+        <v>0</v>
       </c>
       <c r="I24">
-        <v>-15</v>
+        <v>0</v>
       </c>
       <c r="J24">
-        <v>11</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
@@ -1884,28 +1885,28 @@
         <v>51</v>
       </c>
       <c r="C25">
-        <v>782</v>
+        <v>0</v>
       </c>
       <c r="D25">
-        <v>470</v>
+        <v>0</v>
       </c>
       <c r="E25">
-        <v>-3</v>
+        <v>0</v>
       </c>
       <c r="F25">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="G25">
-        <v>-7</v>
+        <v>0</v>
       </c>
       <c r="H25">
-        <v>-28</v>
+        <v>0</v>
       </c>
       <c r="I25">
-        <v>-13</v>
+        <v>0</v>
       </c>
       <c r="J25">
-        <v>9</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
@@ -1915,29 +1916,29 @@
       <c r="B26" t="s">
         <v>53</v>
       </c>
-      <c r="C26" s="1">
-        <v>6098</v>
-      </c>
-      <c r="D26" s="1">
-        <v>3367</v>
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
       </c>
       <c r="E26">
-        <v>-17</v>
+        <v>0</v>
       </c>
       <c r="F26">
-        <v>-7</v>
+        <v>0</v>
       </c>
       <c r="G26">
-        <v>-10</v>
+        <v>0</v>
       </c>
       <c r="H26">
-        <v>-37</v>
+        <v>0</v>
       </c>
       <c r="I26">
-        <v>-19</v>
+        <v>0</v>
       </c>
       <c r="J26">
-        <v>12</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
@@ -1979,29 +1980,29 @@
       <c r="B28" t="s">
         <v>57</v>
       </c>
-      <c r="C28" s="1">
-        <v>3417</v>
-      </c>
-      <c r="D28" s="1">
-        <v>1794</v>
+      <c r="C28">
+        <v>0</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
       </c>
       <c r="E28">
-        <v>-13</v>
+        <v>0</v>
       </c>
       <c r="F28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G28">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H28">
-        <v>-41</v>
+        <v>0</v>
       </c>
       <c r="I28">
-        <v>-19</v>
+        <v>0</v>
       </c>
       <c r="J28">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
@@ -2012,28 +2013,28 @@
         <v>59</v>
       </c>
       <c r="C29">
-        <v>674</v>
+        <v>0</v>
       </c>
       <c r="D29">
-        <v>399</v>
+        <v>0</v>
       </c>
       <c r="E29">
-        <v>-23</v>
+        <v>0</v>
       </c>
       <c r="F29">
-        <v>-17</v>
+        <v>0</v>
       </c>
       <c r="G29">
-        <v>-32</v>
+        <v>0</v>
       </c>
       <c r="H29">
-        <v>-56</v>
+        <v>0</v>
       </c>
       <c r="I29">
-        <v>-29</v>
+        <v>0</v>
       </c>
       <c r="J29">
-        <v>13</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
@@ -2076,28 +2077,28 @@
         <v>63</v>
       </c>
       <c r="C31">
-        <v>387</v>
+        <v>0</v>
       </c>
       <c r="D31">
-        <v>355</v>
+        <v>0</v>
       </c>
       <c r="E31">
-        <v>-23</v>
+        <v>0</v>
       </c>
       <c r="F31">
-        <v>-12</v>
+        <v>0</v>
       </c>
       <c r="G31">
-        <v>-18</v>
+        <v>0</v>
       </c>
       <c r="H31">
-        <v>-36</v>
+        <v>0</v>
       </c>
       <c r="I31">
-        <v>-18</v>
+        <v>0</v>
       </c>
       <c r="J31">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
@@ -2107,29 +2108,29 @@
       <c r="B32" t="s">
         <v>65</v>
       </c>
-      <c r="C32" s="1">
-        <v>2065</v>
-      </c>
-      <c r="D32" s="1">
-        <v>1288</v>
+      <c r="C32">
+        <v>0</v>
+      </c>
+      <c r="D32">
+        <v>0</v>
       </c>
       <c r="E32">
-        <v>-13</v>
+        <v>0</v>
       </c>
       <c r="F32">
-        <v>-4</v>
+        <v>0</v>
       </c>
       <c r="G32">
-        <v>-17</v>
+        <v>0</v>
       </c>
       <c r="H32">
-        <v>-53</v>
+        <v>0</v>
       </c>
       <c r="I32">
-        <v>-15</v>
+        <v>0</v>
       </c>
       <c r="J32">
-        <v>12</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
@@ -2140,28 +2141,28 @@
         <v>67</v>
       </c>
       <c r="C33">
-        <v>433</v>
+        <v>0</v>
       </c>
       <c r="D33">
-        <v>292</v>
+        <v>0</v>
       </c>
       <c r="E33">
-        <v>-20</v>
+        <v>0</v>
       </c>
       <c r="F33">
-        <v>-7</v>
+        <v>0</v>
       </c>
       <c r="G33">
-        <v>-31</v>
+        <v>0</v>
       </c>
       <c r="H33">
-        <v>-47</v>
+        <v>0</v>
       </c>
       <c r="I33">
-        <v>-19</v>
+        <v>0</v>
       </c>
       <c r="J33">
-        <v>11</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
@@ -2172,28 +2173,28 @@
         <v>69</v>
       </c>
       <c r="C34">
-        <v>230</v>
+        <v>0</v>
       </c>
       <c r="D34">
-        <v>140</v>
+        <v>0</v>
       </c>
       <c r="E34">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F34">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="G34">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H34">
-        <v>-29</v>
+        <v>0</v>
       </c>
       <c r="I34">
-        <v>-12</v>
+        <v>0</v>
       </c>
       <c r="J34">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
@@ -2204,28 +2205,28 @@
         <v>71</v>
       </c>
       <c r="C35">
-        <v>948</v>
+        <v>0</v>
       </c>
       <c r="D35">
-        <v>760</v>
+        <v>0</v>
       </c>
       <c r="E35">
-        <v>-7</v>
+        <v>0</v>
       </c>
       <c r="F35">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G35">
-        <v>-9</v>
+        <v>0</v>
       </c>
       <c r="H35">
-        <v>-31</v>
+        <v>0</v>
       </c>
       <c r="I35">
-        <v>-19</v>
+        <v>0</v>
       </c>
       <c r="J35">
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated thresholds for island decision rules, updated historical COVID and policy data, updated geospatial COVID data
</commit_message>
<xml_diff>
--- a/Data/Indonesia/Misc/ShapefileAddingIndonesia.xlsx
+++ b/Data/Indonesia/Misc/ShapefileAddingIndonesia.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20366"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,19 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\slomb\OneDrive\Desktop\SD_UI\Data\Indonesia\Misc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{EDB81CDC-EED2-42A1-A031-C1713B3F03C8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85A9D9BD-3912-4923-B592-166E412C4ED1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="16725"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="16725" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ShapefileAddingIndonesia" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="80">
   <si>
     <t>Province</t>
   </si>
@@ -257,13 +257,16 @@
   </si>
   <si>
     <t>houseex</t>
+  </si>
+  <si>
+    <t>Deaths</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="18" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -398,6 +401,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -580,7 +589,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -695,6 +704,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -740,9 +764,12 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1097,16 +1124,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K35"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:L35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1120,203 +1151,221 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>77</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>9</v>
       </c>
       <c r="B2" t="s">
         <v>10</v>
       </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
-      <c r="I2">
-        <v>0</v>
-      </c>
-      <c r="J2">
-        <v>0</v>
-      </c>
-      <c r="K2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C2" s="2">
+        <v>0</v>
+      </c>
+      <c r="D2" s="2">
+        <v>0</v>
+      </c>
+      <c r="E2" s="2">
+        <v>0</v>
+      </c>
+      <c r="F2" s="2">
+        <v>0</v>
+      </c>
+      <c r="G2" s="2">
+        <v>0</v>
+      </c>
+      <c r="H2" s="2">
+        <v>0</v>
+      </c>
+      <c r="I2" s="2">
+        <v>0</v>
+      </c>
+      <c r="J2" s="2">
+        <v>0</v>
+      </c>
+      <c r="K2" s="2">
+        <v>0</v>
+      </c>
+      <c r="L2" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>11</v>
       </c>
       <c r="B3" t="s">
         <v>12</v>
       </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-      <c r="G3">
-        <v>0</v>
-      </c>
-      <c r="H3">
-        <v>0</v>
-      </c>
-      <c r="I3">
-        <v>0</v>
-      </c>
-      <c r="J3">
-        <v>0</v>
-      </c>
-      <c r="K3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C3" s="2">
+        <v>0</v>
+      </c>
+      <c r="D3" s="2">
+        <v>0</v>
+      </c>
+      <c r="E3" s="2">
+        <v>0</v>
+      </c>
+      <c r="F3" s="2">
+        <v>0</v>
+      </c>
+      <c r="G3" s="2">
+        <v>0</v>
+      </c>
+      <c r="H3" s="2">
+        <v>0</v>
+      </c>
+      <c r="I3" s="2">
+        <v>0</v>
+      </c>
+      <c r="J3" s="2">
+        <v>0</v>
+      </c>
+      <c r="K3" s="2">
+        <v>0</v>
+      </c>
+      <c r="L3" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>13</v>
       </c>
       <c r="B4" t="s">
         <v>14</v>
       </c>
-      <c r="C4">
-        <v>0</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-      <c r="H4">
-        <v>0</v>
-      </c>
-      <c r="I4">
-        <v>0</v>
-      </c>
-      <c r="J4">
-        <v>0</v>
-      </c>
-      <c r="K4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C4" s="2">
+        <v>0</v>
+      </c>
+      <c r="D4" s="2">
+        <v>0</v>
+      </c>
+      <c r="E4" s="2">
+        <v>0</v>
+      </c>
+      <c r="F4" s="2">
+        <v>0</v>
+      </c>
+      <c r="G4" s="2">
+        <v>0</v>
+      </c>
+      <c r="H4" s="2">
+        <v>0</v>
+      </c>
+      <c r="I4" s="2">
+        <v>0</v>
+      </c>
+      <c r="J4" s="2">
+        <v>0</v>
+      </c>
+      <c r="K4" s="2">
+        <v>0</v>
+      </c>
+      <c r="L4" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>15</v>
       </c>
       <c r="B5" t="s">
         <v>16</v>
       </c>
-      <c r="C5">
-        <v>0</v>
-      </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-      <c r="F5">
-        <v>0</v>
-      </c>
-      <c r="G5">
-        <v>0</v>
-      </c>
-      <c r="H5">
-        <v>0</v>
-      </c>
-      <c r="I5">
-        <v>0</v>
-      </c>
-      <c r="J5">
-        <v>0</v>
-      </c>
-      <c r="K5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C5" s="2">
+        <v>0</v>
+      </c>
+      <c r="D5" s="2">
+        <v>0</v>
+      </c>
+      <c r="E5" s="2">
+        <v>0</v>
+      </c>
+      <c r="F5" s="2">
+        <v>0</v>
+      </c>
+      <c r="G5" s="2">
+        <v>0</v>
+      </c>
+      <c r="H5" s="2">
+        <v>0</v>
+      </c>
+      <c r="I5" s="2">
+        <v>0</v>
+      </c>
+      <c r="J5" s="2">
+        <v>0</v>
+      </c>
+      <c r="K5" s="2">
+        <v>0</v>
+      </c>
+      <c r="L5" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>17</v>
       </c>
       <c r="B6" t="s">
         <v>18</v>
       </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
-      <c r="G6">
-        <v>0</v>
-      </c>
-      <c r="H6">
-        <v>0</v>
-      </c>
-      <c r="I6">
-        <v>0</v>
-      </c>
-      <c r="J6">
-        <v>0</v>
-      </c>
-      <c r="K6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C6" s="2">
+        <v>0</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0</v>
+      </c>
+      <c r="E6" s="2">
+        <v>0</v>
+      </c>
+      <c r="F6" s="2">
+        <v>0</v>
+      </c>
+      <c r="G6" s="2">
+        <v>0</v>
+      </c>
+      <c r="H6" s="2">
+        <v>0</v>
+      </c>
+      <c r="I6" s="2">
+        <v>0</v>
+      </c>
+      <c r="J6" s="2">
+        <v>0</v>
+      </c>
+      <c r="K6" s="2">
+        <v>0</v>
+      </c>
+      <c r="L6" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -1324,104 +1373,113 @@
         <v>20</v>
       </c>
       <c r="C7" s="1">
-        <v>9516</v>
+        <v>18451</v>
       </c>
       <c r="D7" s="1">
-        <v>5319</v>
-      </c>
-      <c r="E7">
+        <v>11632</v>
+      </c>
+      <c r="E7" s="1">
+        <v>1179</v>
+      </c>
+      <c r="F7">
         <v>-6</v>
       </c>
-      <c r="F7">
+      <c r="G7">
         <v>1</v>
       </c>
-      <c r="G7">
+      <c r="H7">
         <v>-9</v>
       </c>
-      <c r="H7">
+      <c r="I7">
         <v>-37</v>
       </c>
-      <c r="I7">
+      <c r="J7">
         <v>-18</v>
       </c>
-      <c r="J7">
+      <c r="K7">
         <v>13</v>
       </c>
-      <c r="K7">
+      <c r="L7">
         <v>-4.9292343457456536</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>21</v>
       </c>
       <c r="B8" t="s">
         <v>22</v>
       </c>
-      <c r="C8">
-        <v>0</v>
-      </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="E8">
-        <v>0</v>
-      </c>
-      <c r="F8">
-        <v>0</v>
-      </c>
-      <c r="G8">
-        <v>0</v>
-      </c>
-      <c r="H8">
-        <v>0</v>
-      </c>
-      <c r="I8">
-        <v>0</v>
-      </c>
-      <c r="J8">
-        <v>0</v>
-      </c>
-      <c r="K8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C8" s="2">
+        <v>0</v>
+      </c>
+      <c r="D8" s="2">
+        <v>0</v>
+      </c>
+      <c r="E8" s="2">
+        <v>0</v>
+      </c>
+      <c r="F8" s="2">
+        <v>0</v>
+      </c>
+      <c r="G8" s="2">
+        <v>0</v>
+      </c>
+      <c r="H8" s="2">
+        <v>0</v>
+      </c>
+      <c r="I8" s="2">
+        <v>0</v>
+      </c>
+      <c r="J8" s="2">
+        <v>0</v>
+      </c>
+      <c r="K8" s="2">
+        <v>0</v>
+      </c>
+      <c r="L8" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>23</v>
       </c>
       <c r="B9" t="s">
         <v>24</v>
       </c>
-      <c r="C9">
-        <v>0</v>
-      </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-      <c r="E9">
-        <v>0</v>
-      </c>
-      <c r="F9">
-        <v>0</v>
-      </c>
-      <c r="G9">
-        <v>0</v>
-      </c>
-      <c r="H9">
-        <v>0</v>
-      </c>
-      <c r="I9">
-        <v>0</v>
-      </c>
-      <c r="J9">
-        <v>0</v>
-      </c>
-      <c r="K9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C9" s="2">
+        <v>0</v>
+      </c>
+      <c r="D9" s="2">
+        <v>0</v>
+      </c>
+      <c r="E9" s="2">
+        <v>0</v>
+      </c>
+      <c r="F9" s="2">
+        <v>0</v>
+      </c>
+      <c r="G9" s="2">
+        <v>0</v>
+      </c>
+      <c r="H9" s="2">
+        <v>0</v>
+      </c>
+      <c r="I9" s="2">
+        <v>0</v>
+      </c>
+      <c r="J9" s="2">
+        <v>0</v>
+      </c>
+      <c r="K9" s="2">
+        <v>0</v>
+      </c>
+      <c r="L9" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>25</v>
       </c>
@@ -1429,139 +1487,145 @@
         <v>26</v>
       </c>
       <c r="C10" s="1">
-        <v>22089</v>
+        <v>39181</v>
       </c>
       <c r="D10" s="1">
-        <v>14415</v>
-      </c>
-      <c r="E10">
+        <v>31585</v>
+      </c>
+      <c r="E10" s="1">
+        <v>2867</v>
+      </c>
+      <c r="F10">
         <v>-10</v>
       </c>
-      <c r="F10">
+      <c r="G10">
         <v>-4</v>
       </c>
-      <c r="G10">
+      <c r="H10">
         <v>-14</v>
       </c>
-      <c r="H10">
+      <c r="I10">
         <v>-38</v>
       </c>
-      <c r="I10">
+      <c r="J10">
         <v>-21</v>
       </c>
-      <c r="J10">
+      <c r="K10">
         <v>14</v>
       </c>
-      <c r="K10">
+      <c r="L10">
         <v>-4.8203515127295331</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>27</v>
       </c>
       <c r="B11" t="s">
         <v>28</v>
       </c>
-      <c r="C11">
-        <v>0</v>
-      </c>
-      <c r="D11">
-        <v>0</v>
-      </c>
-      <c r="E11">
-        <v>0</v>
-      </c>
-      <c r="F11">
-        <v>0</v>
-      </c>
-      <c r="G11">
-        <v>0</v>
-      </c>
-      <c r="H11">
-        <v>0</v>
-      </c>
-      <c r="I11">
-        <v>0</v>
-      </c>
-      <c r="J11">
-        <v>0</v>
-      </c>
-      <c r="K11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C11" s="2">
+        <v>0</v>
+      </c>
+      <c r="D11" s="2">
+        <v>0</v>
+      </c>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2">
+        <v>0</v>
+      </c>
+      <c r="G11" s="2">
+        <v>0</v>
+      </c>
+      <c r="H11" s="2">
+        <v>0</v>
+      </c>
+      <c r="I11" s="2">
+        <v>0</v>
+      </c>
+      <c r="J11" s="2">
+        <v>0</v>
+      </c>
+      <c r="K11" s="2">
+        <v>0</v>
+      </c>
+      <c r="L11" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>29</v>
       </c>
       <c r="B12" t="s">
         <v>30</v>
       </c>
-      <c r="C12">
-        <v>0</v>
-      </c>
-      <c r="D12">
-        <v>0</v>
-      </c>
-      <c r="E12">
-        <v>0</v>
-      </c>
-      <c r="F12">
-        <v>0</v>
-      </c>
-      <c r="G12">
-        <v>0</v>
-      </c>
-      <c r="H12">
-        <v>0</v>
-      </c>
-      <c r="I12">
-        <v>0</v>
-      </c>
-      <c r="J12">
-        <v>0</v>
-      </c>
-      <c r="K12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C12" s="2">
+        <v>0</v>
+      </c>
+      <c r="D12" s="2">
+        <v>0</v>
+      </c>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2">
+        <v>0</v>
+      </c>
+      <c r="G12" s="2">
+        <v>0</v>
+      </c>
+      <c r="H12" s="2">
+        <v>0</v>
+      </c>
+      <c r="I12" s="2">
+        <v>0</v>
+      </c>
+      <c r="J12" s="2">
+        <v>0</v>
+      </c>
+      <c r="K12" s="2">
+        <v>0</v>
+      </c>
+      <c r="L12" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>31</v>
       </c>
       <c r="B13" t="s">
         <v>32</v>
       </c>
-      <c r="C13">
-        <v>0</v>
-      </c>
-      <c r="D13">
-        <v>0</v>
-      </c>
-      <c r="E13">
-        <v>0</v>
-      </c>
-      <c r="F13">
-        <v>0</v>
-      </c>
-      <c r="G13">
-        <v>0</v>
-      </c>
-      <c r="H13">
-        <v>0</v>
-      </c>
-      <c r="I13">
-        <v>0</v>
-      </c>
-      <c r="J13">
-        <v>0</v>
-      </c>
-      <c r="K13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C13" s="2">
+        <v>0</v>
+      </c>
+      <c r="D13" s="2">
+        <v>0</v>
+      </c>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2">
+        <v>0</v>
+      </c>
+      <c r="G13" s="2">
+        <v>0</v>
+      </c>
+      <c r="H13" s="2">
+        <v>0</v>
+      </c>
+      <c r="I13" s="2">
+        <v>0</v>
+      </c>
+      <c r="J13" s="2">
+        <v>0</v>
+      </c>
+      <c r="K13" s="2">
+        <v>0</v>
+      </c>
+      <c r="L13" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>33</v>
       </c>
@@ -1569,454 +1633,493 @@
         <v>34</v>
       </c>
       <c r="C14" s="1">
-        <v>21399</v>
+        <v>57469</v>
       </c>
       <c r="D14" s="1">
-        <v>13208</v>
-      </c>
-      <c r="E14">
+        <v>44171</v>
+      </c>
+      <c r="E14" s="1">
+        <v>1481</v>
+      </c>
+      <c r="F14">
         <v>-26</v>
       </c>
-      <c r="F14">
+      <c r="G14">
         <v>-8</v>
       </c>
-      <c r="G14">
+      <c r="H14">
         <v>-71</v>
       </c>
-      <c r="H14">
+      <c r="I14">
         <v>-42</v>
       </c>
-      <c r="I14">
+      <c r="J14">
         <v>-31</v>
       </c>
-      <c r="J14">
+      <c r="K14">
         <v>14</v>
       </c>
-      <c r="K14">
+      <c r="L14">
         <v>-7.5196914542577344</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>35</v>
       </c>
       <c r="B15" t="s">
         <v>36</v>
       </c>
-      <c r="C15">
-        <v>0</v>
-      </c>
-      <c r="D15">
-        <v>0</v>
-      </c>
-      <c r="E15">
-        <v>0</v>
-      </c>
-      <c r="F15">
-        <v>0</v>
-      </c>
-      <c r="G15">
-        <v>0</v>
-      </c>
-      <c r="H15">
-        <v>0</v>
-      </c>
-      <c r="I15">
-        <v>0</v>
-      </c>
-      <c r="J15">
-        <v>0</v>
-      </c>
-      <c r="K15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C15" s="2">
+        <v>0</v>
+      </c>
+      <c r="D15" s="2">
+        <v>0</v>
+      </c>
+      <c r="E15" s="2">
+        <v>0</v>
+      </c>
+      <c r="F15" s="2">
+        <v>0</v>
+      </c>
+      <c r="G15" s="2">
+        <v>0</v>
+      </c>
+      <c r="H15" s="2">
+        <v>0</v>
+      </c>
+      <c r="I15" s="2">
+        <v>0</v>
+      </c>
+      <c r="J15" s="2">
+        <v>0</v>
+      </c>
+      <c r="K15" s="2">
+        <v>0</v>
+      </c>
+      <c r="L15" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>37</v>
       </c>
       <c r="B16" t="s">
         <v>38</v>
       </c>
-      <c r="C16">
-        <v>0</v>
-      </c>
-      <c r="D16">
-        <v>0</v>
-      </c>
-      <c r="E16">
-        <v>0</v>
-      </c>
-      <c r="F16">
-        <v>0</v>
-      </c>
-      <c r="G16">
-        <v>0</v>
-      </c>
-      <c r="H16">
-        <v>0</v>
-      </c>
-      <c r="I16">
-        <v>0</v>
-      </c>
-      <c r="J16">
-        <v>0</v>
-      </c>
-      <c r="K16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C16" s="2">
+        <v>0</v>
+      </c>
+      <c r="D16" s="2">
+        <v>0</v>
+      </c>
+      <c r="E16" s="2">
+        <v>0</v>
+      </c>
+      <c r="F16" s="2">
+        <v>0</v>
+      </c>
+      <c r="G16" s="2">
+        <v>0</v>
+      </c>
+      <c r="H16" s="2">
+        <v>0</v>
+      </c>
+      <c r="I16" s="2">
+        <v>0</v>
+      </c>
+      <c r="J16" s="2">
+        <v>0</v>
+      </c>
+      <c r="K16" s="2">
+        <v>0</v>
+      </c>
+      <c r="L16" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>39</v>
       </c>
       <c r="B17" t="s">
         <v>40</v>
       </c>
-      <c r="C17">
-        <v>0</v>
-      </c>
-      <c r="D17">
-        <v>0</v>
-      </c>
-      <c r="E17">
-        <v>0</v>
-      </c>
-      <c r="F17">
-        <v>0</v>
-      </c>
-      <c r="G17">
-        <v>0</v>
-      </c>
-      <c r="H17">
-        <v>0</v>
-      </c>
-      <c r="I17">
-        <v>0</v>
-      </c>
-      <c r="J17">
-        <v>0</v>
-      </c>
-      <c r="K17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C17" s="2">
+        <v>0</v>
+      </c>
+      <c r="D17" s="2">
+        <v>0</v>
+      </c>
+      <c r="E17" s="2">
+        <v>0</v>
+      </c>
+      <c r="F17" s="2">
+        <v>0</v>
+      </c>
+      <c r="G17" s="2">
+        <v>0</v>
+      </c>
+      <c r="H17" s="2">
+        <v>0</v>
+      </c>
+      <c r="I17" s="2">
+        <v>0</v>
+      </c>
+      <c r="J17" s="2">
+        <v>0</v>
+      </c>
+      <c r="K17" s="2">
+        <v>0</v>
+      </c>
+      <c r="L17" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>41</v>
       </c>
       <c r="B18" t="s">
         <v>42</v>
       </c>
-      <c r="C18">
-        <v>0</v>
-      </c>
-      <c r="D18">
-        <v>0</v>
-      </c>
-      <c r="E18">
-        <v>0</v>
-      </c>
-      <c r="F18">
-        <v>0</v>
-      </c>
-      <c r="G18">
-        <v>0</v>
-      </c>
-      <c r="H18">
-        <v>0</v>
-      </c>
-      <c r="I18">
-        <v>0</v>
-      </c>
-      <c r="J18">
-        <v>0</v>
-      </c>
-      <c r="K18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C18" s="2">
+        <v>0</v>
+      </c>
+      <c r="D18" s="2">
+        <v>0</v>
+      </c>
+      <c r="E18" s="2">
+        <v>0</v>
+      </c>
+      <c r="F18" s="2">
+        <v>0</v>
+      </c>
+      <c r="G18" s="2">
+        <v>0</v>
+      </c>
+      <c r="H18" s="2">
+        <v>0</v>
+      </c>
+      <c r="I18" s="2">
+        <v>0</v>
+      </c>
+      <c r="J18" s="2">
+        <v>0</v>
+      </c>
+      <c r="K18" s="2">
+        <v>0</v>
+      </c>
+      <c r="L18" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>43</v>
       </c>
       <c r="B19" t="s">
         <v>44</v>
       </c>
-      <c r="C19">
-        <v>0</v>
-      </c>
-      <c r="D19">
-        <v>0</v>
-      </c>
-      <c r="E19">
-        <v>0</v>
-      </c>
-      <c r="F19">
-        <v>0</v>
-      </c>
-      <c r="G19">
-        <v>0</v>
-      </c>
-      <c r="H19">
-        <v>0</v>
-      </c>
-      <c r="I19">
-        <v>0</v>
-      </c>
-      <c r="J19">
-        <v>0</v>
-      </c>
-      <c r="K19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C19" s="2">
+        <v>0</v>
+      </c>
+      <c r="D19" s="2">
+        <v>0</v>
+      </c>
+      <c r="E19" s="2">
+        <v>0</v>
+      </c>
+      <c r="F19" s="2">
+        <v>0</v>
+      </c>
+      <c r="G19" s="2">
+        <v>0</v>
+      </c>
+      <c r="H19" s="2">
+        <v>0</v>
+      </c>
+      <c r="I19" s="2">
+        <v>0</v>
+      </c>
+      <c r="J19" s="2">
+        <v>0</v>
+      </c>
+      <c r="K19" s="2">
+        <v>0</v>
+      </c>
+      <c r="L19" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>45</v>
       </c>
       <c r="B20" t="s">
         <v>46</v>
       </c>
-      <c r="C20">
-        <v>0</v>
-      </c>
-      <c r="D20">
-        <v>0</v>
-      </c>
-      <c r="E20">
-        <v>0</v>
-      </c>
-      <c r="F20">
-        <v>0</v>
-      </c>
-      <c r="G20">
-        <v>0</v>
-      </c>
-      <c r="H20">
-        <v>0</v>
-      </c>
-      <c r="I20">
-        <v>0</v>
-      </c>
-      <c r="J20">
-        <v>0</v>
-      </c>
-      <c r="K20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C20" s="2">
+        <v>0</v>
+      </c>
+      <c r="D20" s="2">
+        <v>0</v>
+      </c>
+      <c r="E20" s="2">
+        <v>0</v>
+      </c>
+      <c r="F20" s="2">
+        <v>0</v>
+      </c>
+      <c r="G20" s="2">
+        <v>0</v>
+      </c>
+      <c r="H20" s="2">
+        <v>0</v>
+      </c>
+      <c r="I20" s="2">
+        <v>0</v>
+      </c>
+      <c r="J20" s="2">
+        <v>0</v>
+      </c>
+      <c r="K20" s="2">
+        <v>0</v>
+      </c>
+      <c r="L20" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>47</v>
       </c>
       <c r="B21" t="s">
         <v>48</v>
       </c>
-      <c r="C21">
-        <v>0</v>
-      </c>
-      <c r="D21">
-        <v>0</v>
-      </c>
-      <c r="E21">
-        <v>0</v>
-      </c>
-      <c r="F21">
-        <v>0</v>
-      </c>
-      <c r="G21">
-        <v>0</v>
-      </c>
-      <c r="H21">
-        <v>0</v>
-      </c>
-      <c r="I21">
-        <v>0</v>
-      </c>
-      <c r="J21">
-        <v>0</v>
-      </c>
-      <c r="K21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C21" s="2">
+        <v>0</v>
+      </c>
+      <c r="D21" s="2">
+        <v>0</v>
+      </c>
+      <c r="E21" s="2">
+        <v>0</v>
+      </c>
+      <c r="F21" s="2">
+        <v>0</v>
+      </c>
+      <c r="G21" s="2">
+        <v>0</v>
+      </c>
+      <c r="H21" s="2">
+        <v>0</v>
+      </c>
+      <c r="I21" s="2">
+        <v>0</v>
+      </c>
+      <c r="J21" s="2">
+        <v>0</v>
+      </c>
+      <c r="K21" s="2">
+        <v>0</v>
+      </c>
+      <c r="L21" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>49</v>
       </c>
       <c r="B22" t="s">
         <v>50</v>
       </c>
-      <c r="C22">
-        <v>0</v>
-      </c>
-      <c r="D22">
-        <v>0</v>
-      </c>
-      <c r="E22">
-        <v>0</v>
-      </c>
-      <c r="F22">
-        <v>0</v>
-      </c>
-      <c r="G22">
-        <v>0</v>
-      </c>
-      <c r="H22">
-        <v>0</v>
-      </c>
-      <c r="I22">
-        <v>0</v>
-      </c>
-      <c r="J22">
-        <v>0</v>
-      </c>
-      <c r="K22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C22" s="2">
+        <v>0</v>
+      </c>
+      <c r="D22" s="2">
+        <v>0</v>
+      </c>
+      <c r="E22" s="2">
+        <v>0</v>
+      </c>
+      <c r="F22" s="2">
+        <v>0</v>
+      </c>
+      <c r="G22" s="2">
+        <v>0</v>
+      </c>
+      <c r="H22" s="2">
+        <v>0</v>
+      </c>
+      <c r="I22" s="2">
+        <v>0</v>
+      </c>
+      <c r="J22" s="2">
+        <v>0</v>
+      </c>
+      <c r="K22" s="2">
+        <v>0</v>
+      </c>
+      <c r="L22" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>51</v>
       </c>
       <c r="B23" t="s">
         <v>52</v>
       </c>
-      <c r="C23">
-        <v>0</v>
-      </c>
-      <c r="D23">
-        <v>0</v>
-      </c>
-      <c r="E23">
-        <v>0</v>
-      </c>
-      <c r="F23">
-        <v>0</v>
-      </c>
-      <c r="G23">
-        <v>0</v>
-      </c>
-      <c r="H23">
-        <v>0</v>
-      </c>
-      <c r="I23">
-        <v>0</v>
-      </c>
-      <c r="J23">
-        <v>0</v>
-      </c>
-      <c r="K23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C23" s="2">
+        <v>0</v>
+      </c>
+      <c r="D23" s="2">
+        <v>0</v>
+      </c>
+      <c r="E23" s="2">
+        <v>0</v>
+      </c>
+      <c r="F23" s="2">
+        <v>0</v>
+      </c>
+      <c r="G23" s="2">
+        <v>0</v>
+      </c>
+      <c r="H23" s="2">
+        <v>0</v>
+      </c>
+      <c r="I23" s="2">
+        <v>0</v>
+      </c>
+      <c r="J23" s="2">
+        <v>0</v>
+      </c>
+      <c r="K23" s="2">
+        <v>0</v>
+      </c>
+      <c r="L23" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>53</v>
       </c>
       <c r="B24" t="s">
         <v>54</v>
       </c>
-      <c r="C24">
-        <v>0</v>
-      </c>
-      <c r="D24">
-        <v>0</v>
-      </c>
-      <c r="E24">
-        <v>0</v>
-      </c>
-      <c r="F24">
-        <v>0</v>
-      </c>
-      <c r="G24">
-        <v>0</v>
-      </c>
-      <c r="H24">
-        <v>0</v>
-      </c>
-      <c r="I24">
-        <v>0</v>
-      </c>
-      <c r="J24">
-        <v>0</v>
-      </c>
-      <c r="K24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C24" s="2">
+        <v>0</v>
+      </c>
+      <c r="D24" s="2">
+        <v>0</v>
+      </c>
+      <c r="E24" s="2">
+        <v>0</v>
+      </c>
+      <c r="F24" s="2">
+        <v>0</v>
+      </c>
+      <c r="G24" s="2">
+        <v>0</v>
+      </c>
+      <c r="H24" s="2">
+        <v>0</v>
+      </c>
+      <c r="I24" s="2">
+        <v>0</v>
+      </c>
+      <c r="J24" s="2">
+        <v>0</v>
+      </c>
+      <c r="K24" s="2">
+        <v>0</v>
+      </c>
+      <c r="L24" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>55</v>
       </c>
       <c r="B25" t="s">
         <v>56</v>
       </c>
-      <c r="C25">
-        <v>0</v>
-      </c>
-      <c r="D25">
-        <v>0</v>
-      </c>
-      <c r="E25">
-        <v>0</v>
-      </c>
-      <c r="F25">
-        <v>0</v>
-      </c>
-      <c r="G25">
-        <v>0</v>
-      </c>
-      <c r="H25">
-        <v>0</v>
-      </c>
-      <c r="I25">
-        <v>0</v>
-      </c>
-      <c r="J25">
-        <v>0</v>
-      </c>
-      <c r="K25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C25" s="2">
+        <v>0</v>
+      </c>
+      <c r="D25" s="2">
+        <v>0</v>
+      </c>
+      <c r="E25" s="2">
+        <v>0</v>
+      </c>
+      <c r="F25" s="2">
+        <v>0</v>
+      </c>
+      <c r="G25" s="2">
+        <v>0</v>
+      </c>
+      <c r="H25" s="2">
+        <v>0</v>
+      </c>
+      <c r="I25" s="2">
+        <v>0</v>
+      </c>
+      <c r="J25" s="2">
+        <v>0</v>
+      </c>
+      <c r="K25" s="2">
+        <v>0</v>
+      </c>
+      <c r="L25" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>57</v>
       </c>
       <c r="B26" t="s">
         <v>58</v>
       </c>
-      <c r="C26">
-        <v>0</v>
-      </c>
-      <c r="D26">
-        <v>0</v>
-      </c>
-      <c r="E26">
-        <v>0</v>
-      </c>
-      <c r="F26">
-        <v>0</v>
-      </c>
-      <c r="G26">
-        <v>0</v>
-      </c>
-      <c r="H26">
-        <v>0</v>
-      </c>
-      <c r="I26">
-        <v>0</v>
-      </c>
-      <c r="J26">
-        <v>0</v>
-      </c>
-      <c r="K26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C26" s="2">
+        <v>0</v>
+      </c>
+      <c r="D26" s="2">
+        <v>0</v>
+      </c>
+      <c r="E26" s="2">
+        <v>0</v>
+      </c>
+      <c r="F26" s="2">
+        <v>0</v>
+      </c>
+      <c r="G26" s="2">
+        <v>0</v>
+      </c>
+      <c r="H26" s="2">
+        <v>0</v>
+      </c>
+      <c r="I26" s="2">
+        <v>0</v>
+      </c>
+      <c r="J26" s="2">
+        <v>0</v>
+      </c>
+      <c r="K26" s="2">
+        <v>0</v>
+      </c>
+      <c r="L26" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>59</v>
       </c>
@@ -2024,104 +2127,113 @@
         <v>60</v>
       </c>
       <c r="C27" s="1">
-        <v>9422</v>
+        <v>13747</v>
       </c>
       <c r="D27" s="1">
-        <v>6482</v>
-      </c>
-      <c r="E27">
+        <v>10345</v>
+      </c>
+      <c r="E27" s="1">
+        <v>386</v>
+      </c>
+      <c r="F27">
         <v>-15</v>
       </c>
-      <c r="F27">
+      <c r="G27">
         <v>-2</v>
       </c>
-      <c r="G27">
+      <c r="H27">
         <v>-7</v>
       </c>
-      <c r="H27">
+      <c r="I27">
         <v>-47</v>
       </c>
-      <c r="I27">
+      <c r="J27">
         <v>-25</v>
       </c>
-      <c r="J27">
+      <c r="K27">
         <v>12</v>
       </c>
-      <c r="K27">
+      <c r="L27">
         <v>-6.181305037989234</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>61</v>
       </c>
       <c r="B28" t="s">
         <v>62</v>
       </c>
-      <c r="C28">
-        <v>0</v>
-      </c>
-      <c r="D28">
-        <v>0</v>
-      </c>
-      <c r="E28">
-        <v>0</v>
-      </c>
-      <c r="F28">
-        <v>0</v>
-      </c>
-      <c r="G28">
-        <v>0</v>
-      </c>
-      <c r="H28">
-        <v>0</v>
-      </c>
-      <c r="I28">
-        <v>0</v>
-      </c>
-      <c r="J28">
-        <v>0</v>
-      </c>
-      <c r="K28">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C28" s="2">
+        <v>0</v>
+      </c>
+      <c r="D28" s="2">
+        <v>0</v>
+      </c>
+      <c r="E28" s="2">
+        <v>0</v>
+      </c>
+      <c r="F28" s="2">
+        <v>0</v>
+      </c>
+      <c r="G28" s="2">
+        <v>0</v>
+      </c>
+      <c r="H28" s="2">
+        <v>0</v>
+      </c>
+      <c r="I28" s="2">
+        <v>0</v>
+      </c>
+      <c r="J28" s="2">
+        <v>0</v>
+      </c>
+      <c r="K28" s="2">
+        <v>0</v>
+      </c>
+      <c r="L28" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>63</v>
       </c>
       <c r="B29" t="s">
         <v>64</v>
       </c>
-      <c r="C29">
-        <v>0</v>
-      </c>
-      <c r="D29">
-        <v>0</v>
-      </c>
-      <c r="E29">
-        <v>0</v>
-      </c>
-      <c r="F29">
-        <v>0</v>
-      </c>
-      <c r="G29">
-        <v>0</v>
-      </c>
-      <c r="H29">
-        <v>0</v>
-      </c>
-      <c r="I29">
-        <v>0</v>
-      </c>
-      <c r="J29">
-        <v>0</v>
-      </c>
-      <c r="K29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C29" s="2">
+        <v>0</v>
+      </c>
+      <c r="D29" s="2">
+        <v>0</v>
+      </c>
+      <c r="E29" s="2">
+        <v>0</v>
+      </c>
+      <c r="F29" s="2">
+        <v>0</v>
+      </c>
+      <c r="G29" s="2">
+        <v>0</v>
+      </c>
+      <c r="H29" s="2">
+        <v>0</v>
+      </c>
+      <c r="I29" s="2">
+        <v>0</v>
+      </c>
+      <c r="J29" s="2">
+        <v>0</v>
+      </c>
+      <c r="K29" s="2">
+        <v>0</v>
+      </c>
+      <c r="L29" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>65</v>
       </c>
@@ -2129,205 +2241,223 @@
         <v>66</v>
       </c>
       <c r="C30" s="1">
-        <v>6532</v>
+        <v>15231</v>
       </c>
       <c r="D30" s="1">
-        <v>3966</v>
-      </c>
-      <c r="E30">
+        <v>8319</v>
+      </c>
+      <c r="E30" s="1">
+        <v>306</v>
+      </c>
+      <c r="F30">
         <v>-23</v>
       </c>
-      <c r="F30">
+      <c r="G30">
         <v>3</v>
       </c>
-      <c r="G30">
+      <c r="H30">
         <v>-2</v>
       </c>
-      <c r="H30">
+      <c r="I30">
         <v>-28</v>
       </c>
-      <c r="I30">
+      <c r="J30">
         <v>-23</v>
       </c>
-      <c r="J30">
+      <c r="K30">
         <v>13</v>
       </c>
-      <c r="K30">
+      <c r="L30">
         <v>-6.3433217044006769</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>67</v>
       </c>
       <c r="B31" t="s">
         <v>68</v>
       </c>
-      <c r="C31">
-        <v>0</v>
-      </c>
-      <c r="D31">
-        <v>0</v>
-      </c>
-      <c r="E31">
-        <v>0</v>
-      </c>
-      <c r="F31">
-        <v>0</v>
-      </c>
-      <c r="G31">
-        <v>0</v>
-      </c>
-      <c r="H31">
-        <v>0</v>
-      </c>
-      <c r="I31">
-        <v>0</v>
-      </c>
-      <c r="J31">
-        <v>0</v>
-      </c>
-      <c r="K31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C31" s="2">
+        <v>0</v>
+      </c>
+      <c r="D31" s="2">
+        <v>0</v>
+      </c>
+      <c r="E31" s="2">
+        <v>0</v>
+      </c>
+      <c r="F31" s="2">
+        <v>0</v>
+      </c>
+      <c r="G31" s="2">
+        <v>0</v>
+      </c>
+      <c r="H31" s="2">
+        <v>0</v>
+      </c>
+      <c r="I31" s="2">
+        <v>0</v>
+      </c>
+      <c r="J31" s="2">
+        <v>0</v>
+      </c>
+      <c r="K31" s="2">
+        <v>0</v>
+      </c>
+      <c r="L31" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>69</v>
       </c>
       <c r="B32" t="s">
         <v>70</v>
       </c>
-      <c r="C32">
-        <v>0</v>
-      </c>
-      <c r="D32">
-        <v>0</v>
-      </c>
-      <c r="E32">
-        <v>0</v>
-      </c>
-      <c r="F32">
-        <v>0</v>
-      </c>
-      <c r="G32">
-        <v>0</v>
-      </c>
-      <c r="H32">
-        <v>0</v>
-      </c>
-      <c r="I32">
-        <v>0</v>
-      </c>
-      <c r="J32">
-        <v>0</v>
-      </c>
-      <c r="K32">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C32" s="2">
+        <v>0</v>
+      </c>
+      <c r="D32" s="2">
+        <v>0</v>
+      </c>
+      <c r="E32" s="2">
+        <v>0</v>
+      </c>
+      <c r="F32" s="2">
+        <v>0</v>
+      </c>
+      <c r="G32" s="2">
+        <v>0</v>
+      </c>
+      <c r="H32" s="2">
+        <v>0</v>
+      </c>
+      <c r="I32" s="2">
+        <v>0</v>
+      </c>
+      <c r="J32" s="2">
+        <v>0</v>
+      </c>
+      <c r="K32" s="2">
+        <v>0</v>
+      </c>
+      <c r="L32" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>71</v>
       </c>
       <c r="B33" t="s">
         <v>72</v>
       </c>
-      <c r="C33">
-        <v>0</v>
-      </c>
-      <c r="D33">
-        <v>0</v>
-      </c>
-      <c r="E33">
-        <v>0</v>
-      </c>
-      <c r="F33">
-        <v>0</v>
-      </c>
-      <c r="G33">
-        <v>0</v>
-      </c>
-      <c r="H33">
-        <v>0</v>
-      </c>
-      <c r="I33">
-        <v>0</v>
-      </c>
-      <c r="J33">
-        <v>0</v>
-      </c>
-      <c r="K33">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C33" s="2">
+        <v>0</v>
+      </c>
+      <c r="D33" s="2">
+        <v>0</v>
+      </c>
+      <c r="E33" s="2">
+        <v>0</v>
+      </c>
+      <c r="F33" s="2">
+        <v>0</v>
+      </c>
+      <c r="G33" s="2">
+        <v>0</v>
+      </c>
+      <c r="H33" s="2">
+        <v>0</v>
+      </c>
+      <c r="I33" s="2">
+        <v>0</v>
+      </c>
+      <c r="J33" s="2">
+        <v>0</v>
+      </c>
+      <c r="K33" s="2">
+        <v>0</v>
+      </c>
+      <c r="L33" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>73</v>
       </c>
       <c r="B34" t="s">
         <v>74</v>
       </c>
-      <c r="C34">
-        <v>0</v>
-      </c>
-      <c r="D34">
-        <v>0</v>
-      </c>
-      <c r="E34">
-        <v>0</v>
-      </c>
-      <c r="F34">
-        <v>0</v>
-      </c>
-      <c r="G34">
-        <v>0</v>
-      </c>
-      <c r="H34">
-        <v>0</v>
-      </c>
-      <c r="I34">
-        <v>0</v>
-      </c>
-      <c r="J34">
-        <v>0</v>
-      </c>
-      <c r="K34">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C34" s="2">
+        <v>0</v>
+      </c>
+      <c r="D34" s="2">
+        <v>0</v>
+      </c>
+      <c r="E34" s="2">
+        <v>0</v>
+      </c>
+      <c r="F34" s="2">
+        <v>0</v>
+      </c>
+      <c r="G34" s="2">
+        <v>0</v>
+      </c>
+      <c r="H34" s="2">
+        <v>0</v>
+      </c>
+      <c r="I34" s="2">
+        <v>0</v>
+      </c>
+      <c r="J34" s="2">
+        <v>0</v>
+      </c>
+      <c r="K34" s="2">
+        <v>0</v>
+      </c>
+      <c r="L34" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>75</v>
       </c>
       <c r="B35" t="s">
         <v>76</v>
       </c>
-      <c r="C35">
-        <v>0</v>
-      </c>
-      <c r="D35">
-        <v>0</v>
-      </c>
-      <c r="E35">
-        <v>0</v>
-      </c>
-      <c r="F35">
-        <v>0</v>
-      </c>
-      <c r="G35">
-        <v>0</v>
-      </c>
-      <c r="H35">
-        <v>0</v>
-      </c>
-      <c r="I35">
-        <v>0</v>
-      </c>
-      <c r="J35">
-        <v>0</v>
-      </c>
-      <c r="K35">
+      <c r="C35" s="2">
+        <v>0</v>
+      </c>
+      <c r="D35" s="2">
+        <v>0</v>
+      </c>
+      <c r="E35" s="2">
+        <v>0</v>
+      </c>
+      <c r="F35" s="2">
+        <v>0</v>
+      </c>
+      <c r="G35" s="2">
+        <v>0</v>
+      </c>
+      <c r="H35" s="2">
+        <v>0</v>
+      </c>
+      <c r="I35" s="2">
+        <v>0</v>
+      </c>
+      <c r="J35" s="2">
+        <v>0</v>
+      </c>
+      <c r="K35" s="2">
+        <v>0</v>
+      </c>
+      <c r="L35" s="2">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added conditional statements to change legends on map based on range of values
</commit_message>
<xml_diff>
--- a/Data/Indonesia/Misc/ShapefileAddingIndonesia.xlsx
+++ b/Data/Indonesia/Misc/ShapefileAddingIndonesia.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\slomb\OneDrive\Desktop\SD_UI\Data\Indonesia\Misc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{519AF382-7F12-40D1-AB03-F4CE2B70FF59}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C8BFBF4-F5BD-4B4A-8739-EFBE394937BB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -788,7 +788,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
@@ -837,7 +837,8 @@
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1195,15 +1196,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
       <pane xSplit="1" topLeftCell="H1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="S21" sqref="S21"/>
+      <selection pane="topRight" activeCell="T9" sqref="T9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27.5703125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.140625" style="18"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
@@ -1258,7 +1260,7 @@
       <c r="Q1" t="s">
         <v>84</v>
       </c>
-      <c r="R1" t="s">
+      <c r="R1" s="18" t="s">
         <v>85</v>
       </c>
     </row>
@@ -1314,7 +1316,7 @@
       <c r="Q2">
         <v>0</v>
       </c>
-      <c r="R2" s="15">
+      <c r="R2" s="18">
         <v>0</v>
       </c>
     </row>
@@ -1370,7 +1372,7 @@
       <c r="Q3" s="15">
         <v>0</v>
       </c>
-      <c r="R3" s="15">
+      <c r="R3" s="18">
         <v>0</v>
       </c>
     </row>
@@ -1426,7 +1428,7 @@
       <c r="Q4" s="15">
         <v>0</v>
       </c>
-      <c r="R4" s="15">
+      <c r="R4" s="18">
         <v>0</v>
       </c>
     </row>
@@ -1482,7 +1484,7 @@
       <c r="Q5" s="15">
         <v>0</v>
       </c>
-      <c r="R5" s="15">
+      <c r="R5" s="18">
         <v>0</v>
       </c>
     </row>
@@ -1538,7 +1540,7 @@
       <c r="Q6" s="15">
         <v>0</v>
       </c>
-      <c r="R6" s="15">
+      <c r="R6" s="18">
         <v>0</v>
       </c>
     </row>
@@ -1594,7 +1596,7 @@
       <c r="Q7" s="17">
         <v>11.41</v>
       </c>
-      <c r="R7" s="17">
+      <c r="R7" s="19">
         <v>103.89</v>
       </c>
     </row>
@@ -1650,7 +1652,7 @@
       <c r="Q8" s="15">
         <v>0</v>
       </c>
-      <c r="R8" s="15">
+      <c r="R8" s="18">
         <v>0</v>
       </c>
     </row>
@@ -1706,7 +1708,7 @@
       <c r="Q9" s="15">
         <v>0</v>
       </c>
-      <c r="R9" s="15">
+      <c r="R9" s="18">
         <v>0</v>
       </c>
     </row>
@@ -1762,7 +1764,7 @@
       <c r="Q10" s="17">
         <v>10.199999999999999</v>
       </c>
-      <c r="R10" s="17">
+      <c r="R10" s="19">
         <v>95.41</v>
       </c>
     </row>
@@ -1818,7 +1820,7 @@
       <c r="Q11" s="15">
         <v>0</v>
       </c>
-      <c r="R11" s="15">
+      <c r="R11" s="18">
         <v>0</v>
       </c>
     </row>
@@ -1874,7 +1876,7 @@
       <c r="Q12" s="15">
         <v>0</v>
       </c>
-      <c r="R12" s="15">
+      <c r="R12" s="18">
         <v>0</v>
       </c>
     </row>
@@ -1930,7 +1932,7 @@
       <c r="Q13" s="15">
         <v>0</v>
       </c>
-      <c r="R13" s="15">
+      <c r="R13" s="18">
         <v>0</v>
       </c>
     </row>
@@ -1986,7 +1988,7 @@
       <c r="Q14" s="17">
         <v>4.53</v>
       </c>
-      <c r="R14" s="17">
+      <c r="R14" s="19">
         <v>93.59</v>
       </c>
     </row>
@@ -2042,7 +2044,7 @@
       <c r="Q15" s="15">
         <v>0</v>
       </c>
-      <c r="R15" s="15">
+      <c r="R15" s="18">
         <v>0</v>
       </c>
     </row>
@@ -2098,7 +2100,7 @@
       <c r="Q16" s="15">
         <v>0</v>
       </c>
-      <c r="R16" s="15">
+      <c r="R16" s="18">
         <v>0</v>
       </c>
     </row>
@@ -2154,7 +2156,7 @@
       <c r="Q17" s="15">
         <v>0</v>
       </c>
-      <c r="R17" s="15">
+      <c r="R17" s="18">
         <v>0</v>
       </c>
     </row>
@@ -2210,7 +2212,7 @@
       <c r="Q18" s="15">
         <v>0</v>
       </c>
-      <c r="R18" s="15">
+      <c r="R18" s="18">
         <v>0</v>
       </c>
     </row>
@@ -2266,7 +2268,7 @@
       <c r="Q19" s="15">
         <v>0</v>
       </c>
-      <c r="R19" s="15">
+      <c r="R19" s="18">
         <v>0</v>
       </c>
     </row>
@@ -2322,7 +2324,7 @@
       <c r="Q20" s="15">
         <v>0</v>
       </c>
-      <c r="R20" s="15">
+      <c r="R20" s="18">
         <v>0</v>
       </c>
     </row>
@@ -2378,7 +2380,7 @@
       <c r="Q21" s="15">
         <v>0</v>
       </c>
-      <c r="R21" s="15">
+      <c r="R21" s="18">
         <v>0</v>
       </c>
     </row>
@@ -2434,7 +2436,7 @@
       <c r="Q22" s="15">
         <v>0</v>
       </c>
-      <c r="R22" s="15">
+      <c r="R22" s="18">
         <v>0</v>
       </c>
     </row>
@@ -2490,7 +2492,7 @@
       <c r="Q23" s="15">
         <v>0</v>
       </c>
-      <c r="R23" s="15">
+      <c r="R23" s="18">
         <v>0</v>
       </c>
     </row>
@@ -2546,7 +2548,7 @@
       <c r="Q24" s="15">
         <v>0</v>
       </c>
-      <c r="R24" s="15">
+      <c r="R24" s="18">
         <v>0</v>
       </c>
     </row>
@@ -2602,7 +2604,7 @@
       <c r="Q25" s="15">
         <v>0</v>
       </c>
-      <c r="R25" s="15">
+      <c r="R25" s="18">
         <v>0</v>
       </c>
     </row>
@@ -2658,7 +2660,7 @@
       <c r="Q26" s="15">
         <v>0</v>
       </c>
-      <c r="R26" s="15">
+      <c r="R26" s="18">
         <v>0</v>
       </c>
     </row>
@@ -2770,7 +2772,7 @@
       <c r="Q28" s="15">
         <v>0</v>
       </c>
-      <c r="R28" s="15">
+      <c r="R28" s="18">
         <v>0</v>
       </c>
     </row>
@@ -2826,7 +2828,7 @@
       <c r="Q29" s="15">
         <v>0</v>
       </c>
-      <c r="R29" s="15">
+      <c r="R29" s="18">
         <v>0</v>
       </c>
     </row>
@@ -2882,7 +2884,7 @@
       <c r="Q30" s="17">
         <v>7.88</v>
       </c>
-      <c r="R30" s="17">
+      <c r="R30" s="19">
         <v>101.35</v>
       </c>
     </row>
@@ -2938,7 +2940,7 @@
       <c r="Q31" s="15">
         <v>0</v>
       </c>
-      <c r="R31" s="15">
+      <c r="R31" s="18">
         <v>0</v>
       </c>
     </row>
@@ -2994,7 +2996,7 @@
       <c r="Q32" s="15">
         <v>0</v>
       </c>
-      <c r="R32" s="15">
+      <c r="R32" s="18">
         <v>0</v>
       </c>
     </row>
@@ -3050,7 +3052,7 @@
       <c r="Q33" s="15">
         <v>0</v>
       </c>
-      <c r="R33" s="15">
+      <c r="R33" s="18">
         <v>0</v>
       </c>
     </row>
@@ -3106,7 +3108,7 @@
       <c r="Q34" s="15">
         <v>0</v>
       </c>
-      <c r="R34" s="15">
+      <c r="R34" s="18">
         <v>0</v>
       </c>
     </row>
@@ -3162,7 +3164,7 @@
       <c r="Q35" s="15">
         <v>0</v>
       </c>
-      <c r="R35" s="15">
+      <c r="R35" s="18">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
adding inflation data to Indonesia context
</commit_message>
<xml_diff>
--- a/Data/Indonesia/Misc/ShapefileAddingIndonesia.xlsx
+++ b/Data/Indonesia/Misc/ShapefileAddingIndonesia.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\slomb\OneDrive\Desktop\SD_UI\Data\Indonesia\Misc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0615FF50-279A-4D71-906A-4AA1B5D133D3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10E364D1-4856-4A40-9DE4-590D6C39E257}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="88">
   <si>
     <t>Province</t>
   </si>
@@ -278,6 +278,12 @@
   </si>
   <si>
     <t>FTT</t>
+  </si>
+  <si>
+    <t>IF_val</t>
+  </si>
+  <si>
+    <t>IF_chg</t>
   </si>
 </sst>
 </file>
@@ -788,7 +794,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
@@ -839,6 +845,9 @@
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1194,11 +1203,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R35"/>
+  <dimension ref="A1:T36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="H1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="T9" sqref="T9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="S1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="V21" sqref="V21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1208,7 +1217,7 @@
     <col min="18" max="18" width="9.140625" style="18"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1263,8 +1272,14 @@
       <c r="R1" s="18" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S1" t="s">
+        <v>86</v>
+      </c>
+      <c r="T1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -1319,8 +1334,14 @@
       <c r="R2" s="18">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S2" s="18">
+        <v>0</v>
+      </c>
+      <c r="T2" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -1375,8 +1396,14 @@
       <c r="R3" s="18">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S3" s="18">
+        <v>0</v>
+      </c>
+      <c r="T3" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -1431,8 +1458,14 @@
       <c r="R4" s="18">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S4" s="18">
+        <v>0</v>
+      </c>
+      <c r="T4" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -1487,8 +1520,14 @@
       <c r="R5" s="18">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="S5" s="18">
+        <v>0</v>
+      </c>
+      <c r="T5" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -1543,8 +1582,14 @@
       <c r="R6" s="18">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="S6" s="18">
+        <v>0</v>
+      </c>
+      <c r="T6" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>21</v>
       </c>
@@ -1599,8 +1644,14 @@
       <c r="R7" s="19">
         <v>103.89</v>
       </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S7" s="20">
+        <v>0.04</v>
+      </c>
+      <c r="T7">
+        <v>-0.27999999999999997</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>23</v>
       </c>
@@ -1655,8 +1706,14 @@
       <c r="R8" s="18">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="S8" s="18">
+        <v>0</v>
+      </c>
+      <c r="T8" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>25</v>
       </c>
@@ -1711,8 +1768,14 @@
       <c r="R9" s="18">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="S9" s="18">
+        <v>0</v>
+      </c>
+      <c r="T9" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>27</v>
       </c>
@@ -1767,8 +1830,14 @@
       <c r="R10" s="19">
         <v>95.41</v>
       </c>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S10" s="18">
+        <v>-0.15</v>
+      </c>
+      <c r="T10">
+        <v>7.9999999999999988E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>29</v>
       </c>
@@ -1823,8 +1892,14 @@
       <c r="R11" s="18">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S11" s="18">
+        <v>0</v>
+      </c>
+      <c r="T11" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>31</v>
       </c>
@@ -1879,8 +1954,14 @@
       <c r="R12" s="18">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="S12" s="18">
+        <v>0</v>
+      </c>
+      <c r="T12" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>33</v>
       </c>
@@ -1935,8 +2016,14 @@
       <c r="R13" s="18">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="S13" s="18">
+        <v>0</v>
+      </c>
+      <c r="T13" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>35</v>
       </c>
@@ -1991,8 +2078,14 @@
       <c r="R14" s="19">
         <v>93.59</v>
       </c>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S14" s="20">
+        <v>0.02</v>
+      </c>
+      <c r="T14">
+        <v>-0.06</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>37</v>
       </c>
@@ -2047,8 +2140,14 @@
       <c r="R15" s="18">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S15" s="18">
+        <v>0</v>
+      </c>
+      <c r="T15" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>39</v>
       </c>
@@ -2103,8 +2202,14 @@
       <c r="R16" s="18">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S16" s="18">
+        <v>0</v>
+      </c>
+      <c r="T16" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>41</v>
       </c>
@@ -2159,8 +2264,14 @@
       <c r="R17" s="18">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S17" s="18">
+        <v>0</v>
+      </c>
+      <c r="T17" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>43</v>
       </c>
@@ -2215,8 +2326,14 @@
       <c r="R18" s="18">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S18" s="18">
+        <v>0</v>
+      </c>
+      <c r="T18" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>45</v>
       </c>
@@ -2271,8 +2388,14 @@
       <c r="R19" s="18">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S19" s="18">
+        <v>0</v>
+      </c>
+      <c r="T19" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>47</v>
       </c>
@@ -2327,8 +2450,14 @@
       <c r="R20" s="18">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S20" s="18">
+        <v>0</v>
+      </c>
+      <c r="T20" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>49</v>
       </c>
@@ -2383,8 +2512,14 @@
       <c r="R21" s="18">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S21" s="18">
+        <v>0</v>
+      </c>
+      <c r="T21" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>51</v>
       </c>
@@ -2439,8 +2574,14 @@
       <c r="R22" s="18">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S22" s="18">
+        <v>0</v>
+      </c>
+      <c r="T22" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>53</v>
       </c>
@@ -2495,8 +2636,14 @@
       <c r="R23" s="18">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S23" s="18">
+        <v>0</v>
+      </c>
+      <c r="T23" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>55</v>
       </c>
@@ -2551,8 +2698,14 @@
       <c r="R24" s="18">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S24" s="18">
+        <v>0</v>
+      </c>
+      <c r="T24" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>57</v>
       </c>
@@ -2607,8 +2760,14 @@
       <c r="R25" s="18">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="S25" s="18">
+        <v>0</v>
+      </c>
+      <c r="T25" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>59</v>
       </c>
@@ -2663,8 +2822,14 @@
       <c r="R26" s="18">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="S26" s="18">
+        <v>0</v>
+      </c>
+      <c r="T26" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>61</v>
       </c>
@@ -2719,8 +2884,14 @@
       <c r="R27" s="18">
         <v>101.81</v>
       </c>
-    </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S27" s="20">
+        <v>0.02</v>
+      </c>
+      <c r="T27">
+        <v>-0.16999999999999998</v>
+      </c>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>63</v>
       </c>
@@ -2775,8 +2946,14 @@
       <c r="R28" s="18">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="S28" s="18">
+        <v>0</v>
+      </c>
+      <c r="T28" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>65</v>
       </c>
@@ -2831,8 +3008,14 @@
       <c r="R29" s="18">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="S29" s="18">
+        <v>0</v>
+      </c>
+      <c r="T29" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>67</v>
       </c>
@@ -2887,8 +3070,14 @@
       <c r="R30" s="19">
         <v>101.35</v>
       </c>
-    </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S30" s="20">
+        <v>-0.01</v>
+      </c>
+      <c r="T30">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>69</v>
       </c>
@@ -2943,8 +3132,14 @@
       <c r="R31" s="18">
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S31" s="18">
+        <v>0</v>
+      </c>
+      <c r="T31" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>71</v>
       </c>
@@ -2999,8 +3194,14 @@
       <c r="R32" s="18">
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S32" s="18">
+        <v>0</v>
+      </c>
+      <c r="T32" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>73</v>
       </c>
@@ -3055,8 +3256,14 @@
       <c r="R33" s="18">
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S33" s="18">
+        <v>0</v>
+      </c>
+      <c r="T33" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>75</v>
       </c>
@@ -3111,8 +3318,14 @@
       <c r="R34" s="18">
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S34" s="18">
+        <v>0</v>
+      </c>
+      <c r="T34" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>77</v>
       </c>
@@ -3167,6 +3380,16 @@
       <c r="R35" s="18">
         <v>0</v>
       </c>
+      <c r="S35" s="18">
+        <v>0</v>
+      </c>
+      <c r="T35" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="S36" s="18"/>
+      <c r="T36" s="18"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
committing new Indonesian data
</commit_message>
<xml_diff>
--- a/Data/Indonesia/Misc/ShapefileAddingIndonesia.xlsx
+++ b/Data/Indonesia/Misc/ShapefileAddingIndonesia.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\slomb\OneDrive\Desktop\SD_UI\Data\Indonesia\Misc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C8BFBF4-F5BD-4B4A-8739-EFBE394937BB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10E364D1-4856-4A40-9DE4-590D6C39E257}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="88">
   <si>
     <t>Province</t>
   </si>
@@ -278,6 +278,12 @@
   </si>
   <si>
     <t>FTT</t>
+  </si>
+  <si>
+    <t>IF_val</t>
+  </si>
+  <si>
+    <t>IF_chg</t>
   </si>
 </sst>
 </file>
@@ -788,7 +794,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
@@ -839,6 +845,9 @@
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1194,11 +1203,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R35"/>
+  <dimension ref="A1:T36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="H1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="T9" sqref="T9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="S1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="V21" sqref="V21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1208,7 +1217,7 @@
     <col min="18" max="18" width="9.140625" style="18"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1263,8 +1272,14 @@
       <c r="R1" s="18" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S1" t="s">
+        <v>86</v>
+      </c>
+      <c r="T1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -1319,8 +1334,14 @@
       <c r="R2" s="18">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S2" s="18">
+        <v>0</v>
+      </c>
+      <c r="T2" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -1375,8 +1396,14 @@
       <c r="R3" s="18">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S3" s="18">
+        <v>0</v>
+      </c>
+      <c r="T3" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -1431,8 +1458,14 @@
       <c r="R4" s="18">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S4" s="18">
+        <v>0</v>
+      </c>
+      <c r="T4" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -1487,8 +1520,14 @@
       <c r="R5" s="18">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="S5" s="18">
+        <v>0</v>
+      </c>
+      <c r="T5" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -1543,8 +1582,14 @@
       <c r="R6" s="18">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="S6" s="18">
+        <v>0</v>
+      </c>
+      <c r="T6" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>21</v>
       </c>
@@ -1599,8 +1644,14 @@
       <c r="R7" s="19">
         <v>103.89</v>
       </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S7" s="20">
+        <v>0.04</v>
+      </c>
+      <c r="T7">
+        <v>-0.27999999999999997</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>23</v>
       </c>
@@ -1655,8 +1706,14 @@
       <c r="R8" s="18">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="S8" s="18">
+        <v>0</v>
+      </c>
+      <c r="T8" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>25</v>
       </c>
@@ -1711,8 +1768,14 @@
       <c r="R9" s="18">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="S9" s="18">
+        <v>0</v>
+      </c>
+      <c r="T9" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>27</v>
       </c>
@@ -1767,8 +1830,14 @@
       <c r="R10" s="19">
         <v>95.41</v>
       </c>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S10" s="18">
+        <v>-0.15</v>
+      </c>
+      <c r="T10">
+        <v>7.9999999999999988E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>29</v>
       </c>
@@ -1823,8 +1892,14 @@
       <c r="R11" s="18">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S11" s="18">
+        <v>0</v>
+      </c>
+      <c r="T11" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>31</v>
       </c>
@@ -1879,8 +1954,14 @@
       <c r="R12" s="18">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="S12" s="18">
+        <v>0</v>
+      </c>
+      <c r="T12" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>33</v>
       </c>
@@ -1935,8 +2016,14 @@
       <c r="R13" s="18">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="S13" s="18">
+        <v>0</v>
+      </c>
+      <c r="T13" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>35</v>
       </c>
@@ -1991,8 +2078,14 @@
       <c r="R14" s="19">
         <v>93.59</v>
       </c>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S14" s="20">
+        <v>0.02</v>
+      </c>
+      <c r="T14">
+        <v>-0.06</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>37</v>
       </c>
@@ -2047,8 +2140,14 @@
       <c r="R15" s="18">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S15" s="18">
+        <v>0</v>
+      </c>
+      <c r="T15" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>39</v>
       </c>
@@ -2103,8 +2202,14 @@
       <c r="R16" s="18">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S16" s="18">
+        <v>0</v>
+      </c>
+      <c r="T16" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>41</v>
       </c>
@@ -2159,8 +2264,14 @@
       <c r="R17" s="18">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S17" s="18">
+        <v>0</v>
+      </c>
+      <c r="T17" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>43</v>
       </c>
@@ -2215,8 +2326,14 @@
       <c r="R18" s="18">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S18" s="18">
+        <v>0</v>
+      </c>
+      <c r="T18" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>45</v>
       </c>
@@ -2271,8 +2388,14 @@
       <c r="R19" s="18">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S19" s="18">
+        <v>0</v>
+      </c>
+      <c r="T19" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>47</v>
       </c>
@@ -2327,8 +2450,14 @@
       <c r="R20" s="18">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S20" s="18">
+        <v>0</v>
+      </c>
+      <c r="T20" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>49</v>
       </c>
@@ -2383,8 +2512,14 @@
       <c r="R21" s="18">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S21" s="18">
+        <v>0</v>
+      </c>
+      <c r="T21" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>51</v>
       </c>
@@ -2439,8 +2574,14 @@
       <c r="R22" s="18">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S22" s="18">
+        <v>0</v>
+      </c>
+      <c r="T22" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>53</v>
       </c>
@@ -2495,8 +2636,14 @@
       <c r="R23" s="18">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S23" s="18">
+        <v>0</v>
+      </c>
+      <c r="T23" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>55</v>
       </c>
@@ -2551,8 +2698,14 @@
       <c r="R24" s="18">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S24" s="18">
+        <v>0</v>
+      </c>
+      <c r="T24" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>57</v>
       </c>
@@ -2607,8 +2760,14 @@
       <c r="R25" s="18">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="S25" s="18">
+        <v>0</v>
+      </c>
+      <c r="T25" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>59</v>
       </c>
@@ -2663,8 +2822,14 @@
       <c r="R26" s="18">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="S26" s="18">
+        <v>0</v>
+      </c>
+      <c r="T26" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>61</v>
       </c>
@@ -2719,8 +2884,14 @@
       <c r="R27" s="18">
         <v>101.81</v>
       </c>
-    </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S27" s="20">
+        <v>0.02</v>
+      </c>
+      <c r="T27">
+        <v>-0.16999999999999998</v>
+      </c>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>63</v>
       </c>
@@ -2775,8 +2946,14 @@
       <c r="R28" s="18">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="S28" s="18">
+        <v>0</v>
+      </c>
+      <c r="T28" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>65</v>
       </c>
@@ -2831,8 +3008,14 @@
       <c r="R29" s="18">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="S29" s="18">
+        <v>0</v>
+      </c>
+      <c r="T29" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>67</v>
       </c>
@@ -2887,8 +3070,14 @@
       <c r="R30" s="19">
         <v>101.35</v>
       </c>
-    </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S30" s="20">
+        <v>-0.01</v>
+      </c>
+      <c r="T30">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>69</v>
       </c>
@@ -2943,8 +3132,14 @@
       <c r="R31" s="18">
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S31" s="18">
+        <v>0</v>
+      </c>
+      <c r="T31" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>71</v>
       </c>
@@ -2999,8 +3194,14 @@
       <c r="R32" s="18">
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S32" s="18">
+        <v>0</v>
+      </c>
+      <c r="T32" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>73</v>
       </c>
@@ -3055,8 +3256,14 @@
       <c r="R33" s="18">
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S33" s="18">
+        <v>0</v>
+      </c>
+      <c r="T33" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>75</v>
       </c>
@@ -3111,8 +3318,14 @@
       <c r="R34" s="18">
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S34" s="18">
+        <v>0</v>
+      </c>
+      <c r="T34" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>77</v>
       </c>
@@ -3167,6 +3380,16 @@
       <c r="R35" s="18">
         <v>0</v>
       </c>
+      <c r="S35" s="18">
+        <v>0</v>
+      </c>
+      <c r="T35" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="S36" s="18"/>
+      <c r="T36" s="18"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Adding back in changes that for some reason didn't make it when I recloned the reposity for the 64-bit python install. Also adding new categories for economic data to clean up menus
</commit_message>
<xml_diff>
--- a/Data/Indonesia/Misc/ShapefileAddingIndonesia.xlsx
+++ b/Data/Indonesia/Misc/ShapefileAddingIndonesia.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\slomb\OneDrive\Desktop\SD_UI\Data\Indonesia\Misc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10E364D1-4856-4A40-9DE4-590D6C39E257}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA5185C6-D8B7-4372-AAB6-FD3BF9F8CD20}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="90">
   <si>
     <t>Province</t>
   </si>
@@ -284,6 +284,12 @@
   </si>
   <si>
     <t>IF_chg</t>
+  </si>
+  <si>
+    <t>DF_chg</t>
+  </si>
+  <si>
+    <t>HO_chg</t>
   </si>
 </sst>
 </file>
@@ -1203,11 +1209,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T36"/>
+  <dimension ref="A1:V36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="S1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="V21" sqref="V21"/>
+      <selection pane="topRight" activeCell="X34" sqref="X34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1217,7 +1223,7 @@
     <col min="18" max="18" width="9.140625" style="18"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1278,8 +1284,14 @@
       <c r="T1" t="s">
         <v>87</v>
       </c>
+      <c r="U1" t="s">
+        <v>88</v>
+      </c>
+      <c r="V1" t="s">
+        <v>89</v>
+      </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -1340,8 +1352,14 @@
       <c r="T2" s="18">
         <v>0</v>
       </c>
+      <c r="U2" s="18">
+        <v>0</v>
+      </c>
+      <c r="V2" s="18">
+        <v>0</v>
+      </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -1402,8 +1420,14 @@
       <c r="T3" s="18">
         <v>0</v>
       </c>
+      <c r="U3" s="18">
+        <v>0</v>
+      </c>
+      <c r="V3" s="18">
+        <v>0</v>
+      </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -1464,8 +1488,14 @@
       <c r="T4" s="18">
         <v>0</v>
       </c>
+      <c r="U4" s="18">
+        <v>0</v>
+      </c>
+      <c r="V4" s="18">
+        <v>0</v>
+      </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -1526,8 +1556,14 @@
       <c r="T5" s="18">
         <v>0</v>
       </c>
+      <c r="U5" s="18">
+        <v>0</v>
+      </c>
+      <c r="V5" s="18">
+        <v>0</v>
+      </c>
     </row>
-    <row r="6" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -1588,8 +1624,14 @@
       <c r="T6" s="18">
         <v>0</v>
       </c>
+      <c r="U6" s="18">
+        <v>0</v>
+      </c>
+      <c r="V6" s="18">
+        <v>0</v>
+      </c>
     </row>
-    <row r="7" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>21</v>
       </c>
@@ -1650,8 +1692,14 @@
       <c r="T7">
         <v>-0.27999999999999997</v>
       </c>
+      <c r="U7" s="18">
+        <v>0</v>
+      </c>
+      <c r="V7">
+        <v>-35.946843853820596</v>
+      </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>23</v>
       </c>
@@ -1712,8 +1760,14 @@
       <c r="T8" s="18">
         <v>0</v>
       </c>
+      <c r="U8" s="18">
+        <v>0</v>
+      </c>
+      <c r="V8" s="18">
+        <v>0</v>
+      </c>
     </row>
-    <row r="9" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>25</v>
       </c>
@@ -1774,8 +1828,14 @@
       <c r="T9" s="18">
         <v>0</v>
       </c>
+      <c r="U9" s="18">
+        <v>0</v>
+      </c>
+      <c r="V9" s="18">
+        <v>0</v>
+      </c>
     </row>
-    <row r="10" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>27</v>
       </c>
@@ -1836,8 +1896,14 @@
       <c r="T10">
         <v>7.9999999999999988E-2</v>
       </c>
+      <c r="U10" s="18">
+        <v>-65.550286084840735</v>
+      </c>
+      <c r="V10">
+        <v>-37.291246100201867</v>
+      </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>29</v>
       </c>
@@ -1898,8 +1964,14 @@
       <c r="T11" s="18">
         <v>0</v>
       </c>
+      <c r="U11" s="18">
+        <v>0</v>
+      </c>
+      <c r="V11" s="18">
+        <v>0</v>
+      </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>31</v>
       </c>
@@ -1960,8 +2032,14 @@
       <c r="T12" s="18">
         <v>0</v>
       </c>
+      <c r="U12" s="18">
+        <v>0</v>
+      </c>
+      <c r="V12" s="18">
+        <v>0</v>
+      </c>
     </row>
-    <row r="13" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>33</v>
       </c>
@@ -2022,8 +2100,14 @@
       <c r="T13" s="18">
         <v>0</v>
       </c>
+      <c r="U13" s="18">
+        <v>0</v>
+      </c>
+      <c r="V13" s="18">
+        <v>0</v>
+      </c>
     </row>
-    <row r="14" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>35</v>
       </c>
@@ -2084,8 +2168,14 @@
       <c r="T14">
         <v>-0.06</v>
       </c>
+      <c r="U14">
+        <v>-66.488825953857457</v>
+      </c>
+      <c r="V14">
+        <v>-37.738771295818275</v>
+      </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>37</v>
       </c>
@@ -2146,8 +2236,14 @@
       <c r="T15" s="18">
         <v>0</v>
       </c>
+      <c r="U15" s="18">
+        <v>0</v>
+      </c>
+      <c r="V15" s="18">
+        <v>0</v>
+      </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>39</v>
       </c>
@@ -2208,8 +2304,14 @@
       <c r="T16" s="18">
         <v>0</v>
       </c>
+      <c r="U16" s="18">
+        <v>0</v>
+      </c>
+      <c r="V16" s="18">
+        <v>0</v>
+      </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>41</v>
       </c>
@@ -2270,8 +2372,14 @@
       <c r="T17" s="18">
         <v>0</v>
       </c>
+      <c r="U17" s="18">
+        <v>0</v>
+      </c>
+      <c r="V17" s="18">
+        <v>0</v>
+      </c>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>43</v>
       </c>
@@ -2332,8 +2440,14 @@
       <c r="T18" s="18">
         <v>0</v>
       </c>
+      <c r="U18" s="18">
+        <v>0</v>
+      </c>
+      <c r="V18" s="18">
+        <v>0</v>
+      </c>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>45</v>
       </c>
@@ -2394,8 +2508,14 @@
       <c r="T19" s="18">
         <v>0</v>
       </c>
+      <c r="U19" s="18">
+        <v>0</v>
+      </c>
+      <c r="V19" s="18">
+        <v>0</v>
+      </c>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>47</v>
       </c>
@@ -2456,8 +2576,14 @@
       <c r="T20" s="18">
         <v>0</v>
       </c>
+      <c r="U20" s="18">
+        <v>0</v>
+      </c>
+      <c r="V20" s="18">
+        <v>0</v>
+      </c>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>49</v>
       </c>
@@ -2518,8 +2644,14 @@
       <c r="T21" s="18">
         <v>0</v>
       </c>
+      <c r="U21" s="18">
+        <v>0</v>
+      </c>
+      <c r="V21" s="18">
+        <v>0</v>
+      </c>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>51</v>
       </c>
@@ -2580,8 +2712,14 @@
       <c r="T22" s="18">
         <v>0</v>
       </c>
+      <c r="U22" s="18">
+        <v>0</v>
+      </c>
+      <c r="V22" s="18">
+        <v>0</v>
+      </c>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>53</v>
       </c>
@@ -2642,8 +2780,14 @@
       <c r="T23" s="18">
         <v>0</v>
       </c>
+      <c r="U23" s="18">
+        <v>0</v>
+      </c>
+      <c r="V23" s="18">
+        <v>0</v>
+      </c>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>55</v>
       </c>
@@ -2704,8 +2848,14 @@
       <c r="T24" s="18">
         <v>0</v>
       </c>
+      <c r="U24" s="18">
+        <v>0</v>
+      </c>
+      <c r="V24" s="18">
+        <v>0</v>
+      </c>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>57</v>
       </c>
@@ -2766,8 +2916,14 @@
       <c r="T25" s="18">
         <v>0</v>
       </c>
+      <c r="U25" s="18">
+        <v>0</v>
+      </c>
+      <c r="V25" s="18">
+        <v>0</v>
+      </c>
     </row>
-    <row r="26" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>59</v>
       </c>
@@ -2828,8 +2984,14 @@
       <c r="T26" s="18">
         <v>0</v>
       </c>
+      <c r="U26" s="18">
+        <v>0</v>
+      </c>
+      <c r="V26" s="18">
+        <v>0</v>
+      </c>
     </row>
-    <row r="27" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>61</v>
       </c>
@@ -2890,8 +3052,14 @@
       <c r="T27">
         <v>-0.16999999999999998</v>
       </c>
+      <c r="U27">
+        <v>-54.007451575054375</v>
+      </c>
+      <c r="V27">
+        <v>-5.6249999999999982</v>
+      </c>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>63</v>
       </c>
@@ -2952,8 +3120,14 @@
       <c r="T28" s="18">
         <v>0</v>
       </c>
+      <c r="U28" s="18">
+        <v>0</v>
+      </c>
+      <c r="V28" s="18">
+        <v>0</v>
+      </c>
     </row>
-    <row r="29" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>65</v>
       </c>
@@ -3014,8 +3188,14 @@
       <c r="T29" s="18">
         <v>0</v>
       </c>
+      <c r="U29" s="18">
+        <v>0</v>
+      </c>
+      <c r="V29" s="18">
+        <v>0</v>
+      </c>
     </row>
-    <row r="30" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>67</v>
       </c>
@@ -3076,8 +3256,14 @@
       <c r="T30">
         <v>0.25</v>
       </c>
+      <c r="U30" s="18">
+        <v>0</v>
+      </c>
+      <c r="V30">
+        <v>-17.668414683340053</v>
+      </c>
     </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>69</v>
       </c>
@@ -3138,8 +3324,14 @@
       <c r="T31" s="18">
         <v>0</v>
       </c>
+      <c r="U31" s="18">
+        <v>0</v>
+      </c>
+      <c r="V31" s="18">
+        <v>0</v>
+      </c>
     </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>71</v>
       </c>
@@ -3200,8 +3392,14 @@
       <c r="T32" s="18">
         <v>0</v>
       </c>
+      <c r="U32" s="18">
+        <v>0</v>
+      </c>
+      <c r="V32" s="18">
+        <v>0</v>
+      </c>
     </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>73</v>
       </c>
@@ -3262,8 +3460,14 @@
       <c r="T33" s="18">
         <v>0</v>
       </c>
+      <c r="U33" s="18">
+        <v>0</v>
+      </c>
+      <c r="V33" s="18">
+        <v>0</v>
+      </c>
     </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>75</v>
       </c>
@@ -3324,8 +3528,14 @@
       <c r="T34" s="18">
         <v>0</v>
       </c>
+      <c r="U34" s="18">
+        <v>0</v>
+      </c>
+      <c r="V34" s="18">
+        <v>0</v>
+      </c>
     </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>77</v>
       </c>
@@ -3386,8 +3596,14 @@
       <c r="T35" s="18">
         <v>0</v>
       </c>
+      <c r="U35" s="18">
+        <v>0</v>
+      </c>
+      <c r="V35" s="18">
+        <v>0</v>
+      </c>
     </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:22" x14ac:dyDescent="0.25">
       <c r="S36" s="18"/>
       <c r="T36" s="18"/>
     </row>

</xml_diff>

<commit_message>
Adding QIII economic data to Indonesia shapefile
</commit_message>
<xml_diff>
--- a/Data/Indonesia/Misc/ShapefileAddingIndonesia.xlsx
+++ b/Data/Indonesia/Misc/ShapefileAddingIndonesia.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20367"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\slomb\OneDrive\Desktop\SD_UI\Data\Indonesia\Misc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\slomb\OneDrive\Desktop\Vida_Modeling\Data\Indonesia\Misc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA5185C6-D8B7-4372-AAB6-FD3BF9F8CD20}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{B00A4836-DDB3-40AA-B597-0123B4A33EE0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="16725"/>
   </bookViews>
   <sheets>
     <sheet name="ShapefileAddingIndonesia" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -34,6 +34,9 @@
     <t>Recovered</t>
   </si>
   <si>
+    <t>Deaths</t>
+  </si>
+  <si>
     <t>Retail</t>
   </si>
   <si>
@@ -55,6 +58,36 @@
     <t>houseex</t>
   </si>
   <si>
+    <t>consumex</t>
+  </si>
+  <si>
+    <t>govex</t>
+  </si>
+  <si>
+    <t>netex</t>
+  </si>
+  <si>
+    <t>GDRP</t>
+  </si>
+  <si>
+    <t>pov</t>
+  </si>
+  <si>
+    <t>FTT</t>
+  </si>
+  <si>
+    <t>IF_val</t>
+  </si>
+  <si>
+    <t>IF_chg</t>
+  </si>
+  <si>
+    <t>DF_chg</t>
+  </si>
+  <si>
+    <t>HO_chg</t>
+  </si>
+  <si>
     <t>Aceh</t>
   </si>
   <si>
@@ -257,45 +290,12 @@
   </si>
   <si>
     <t>ID-SB</t>
-  </si>
-  <si>
-    <t>govex</t>
-  </si>
-  <si>
-    <t>consumex</t>
-  </si>
-  <si>
-    <t>netex</t>
-  </si>
-  <si>
-    <t>GDRP</t>
-  </si>
-  <si>
-    <t>Deaths</t>
-  </si>
-  <si>
-    <t>pov</t>
-  </si>
-  <si>
-    <t>FTT</t>
-  </si>
-  <si>
-    <t>IF_val</t>
-  </si>
-  <si>
-    <t>IF_chg</t>
-  </si>
-  <si>
-    <t>DF_chg</t>
-  </si>
-  <si>
-    <t>HO_chg</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -432,13 +432,14 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -618,12 +619,6 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00B050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="11">
     <border>
@@ -742,16 +737,16 @@
     </border>
     <border>
       <left style="medium">
-        <color rgb="FFCCCCCC"/>
+        <color rgb="FFA3A3A3"/>
       </left>
       <right style="medium">
-        <color rgb="FFCCCCCC"/>
+        <color rgb="FFA3A3A3"/>
       </right>
       <top style="medium">
-        <color rgb="FFCCCCCC"/>
+        <color rgb="FFA3A3A3"/>
       </top>
       <bottom style="medium">
-        <color rgb="FFCCCCCC"/>
+        <color rgb="FFA3A3A3"/>
       </bottom>
       <diagonal/>
     </border>
@@ -800,60 +795,12 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1208,19 +1155,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:V36"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:V35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="S1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="X34" sqref="X34"/>
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.140625" style="18"/>
+    <col min="2" max="2" width="9" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="6.140625" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="13" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.25">
@@ -1237,66 +1193,66 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>83</v>
+        <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="J1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="K1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="L1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="M1" t="s">
-        <v>80</v>
+        <v>12</v>
       </c>
       <c r="N1" t="s">
-        <v>79</v>
+        <v>13</v>
       </c>
       <c r="O1" t="s">
-        <v>81</v>
+        <v>14</v>
       </c>
       <c r="P1" t="s">
-        <v>82</v>
+        <v>15</v>
       </c>
       <c r="Q1" t="s">
-        <v>84</v>
-      </c>
-      <c r="R1" s="18" t="s">
-        <v>85</v>
+        <v>16</v>
+      </c>
+      <c r="R1" t="s">
+        <v>17</v>
       </c>
       <c r="S1" t="s">
-        <v>86</v>
+        <v>18</v>
       </c>
       <c r="T1" t="s">
-        <v>87</v>
+        <v>19</v>
       </c>
       <c r="U1" t="s">
-        <v>88</v>
+        <v>20</v>
       </c>
       <c r="V1" t="s">
-        <v>89</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -1304,7 +1260,7 @@
       <c r="D2">
         <v>0</v>
       </c>
-      <c r="E2" s="15">
+      <c r="E2">
         <v>0</v>
       </c>
       <c r="F2">
@@ -1343,28 +1299,28 @@
       <c r="Q2">
         <v>0</v>
       </c>
-      <c r="R2" s="18">
-        <v>0</v>
-      </c>
-      <c r="S2" s="18">
-        <v>0</v>
-      </c>
-      <c r="T2" s="18">
-        <v>0</v>
-      </c>
-      <c r="U2" s="18">
-        <v>0</v>
-      </c>
-      <c r="V2" s="18">
+      <c r="R2">
+        <v>0</v>
+      </c>
+      <c r="S2">
+        <v>0</v>
+      </c>
+      <c r="T2">
+        <v>0</v>
+      </c>
+      <c r="U2">
+        <v>0</v>
+      </c>
+      <c r="V2">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -1372,7 +1328,7 @@
       <c r="D3">
         <v>0</v>
       </c>
-      <c r="E3" s="15">
+      <c r="E3">
         <v>0</v>
       </c>
       <c r="F3">
@@ -1408,31 +1364,31 @@
       <c r="P3">
         <v>0</v>
       </c>
-      <c r="Q3" s="15">
-        <v>0</v>
-      </c>
-      <c r="R3" s="18">
-        <v>0</v>
-      </c>
-      <c r="S3" s="18">
-        <v>0</v>
-      </c>
-      <c r="T3" s="18">
-        <v>0</v>
-      </c>
-      <c r="U3" s="18">
-        <v>0</v>
-      </c>
-      <c r="V3" s="18">
+      <c r="Q3">
+        <v>0</v>
+      </c>
+      <c r="R3">
+        <v>0</v>
+      </c>
+      <c r="S3">
+        <v>0</v>
+      </c>
+      <c r="T3">
+        <v>0</v>
+      </c>
+      <c r="U3">
+        <v>0</v>
+      </c>
+      <c r="V3">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -1440,7 +1396,7 @@
       <c r="D4">
         <v>0</v>
       </c>
-      <c r="E4" s="15">
+      <c r="E4">
         <v>0</v>
       </c>
       <c r="F4">
@@ -1476,31 +1432,31 @@
       <c r="P4">
         <v>0</v>
       </c>
-      <c r="Q4" s="15">
-        <v>0</v>
-      </c>
-      <c r="R4" s="18">
-        <v>0</v>
-      </c>
-      <c r="S4" s="18">
-        <v>0</v>
-      </c>
-      <c r="T4" s="18">
-        <v>0</v>
-      </c>
-      <c r="U4" s="18">
-        <v>0</v>
-      </c>
-      <c r="V4" s="18">
+      <c r="Q4">
+        <v>0</v>
+      </c>
+      <c r="R4">
+        <v>0</v>
+      </c>
+      <c r="S4">
+        <v>0</v>
+      </c>
+      <c r="T4">
+        <v>0</v>
+      </c>
+      <c r="U4">
+        <v>0</v>
+      </c>
+      <c r="V4">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -1508,7 +1464,7 @@
       <c r="D5">
         <v>0</v>
       </c>
-      <c r="E5" s="15">
+      <c r="E5">
         <v>0</v>
       </c>
       <c r="F5">
@@ -1544,31 +1500,31 @@
       <c r="P5">
         <v>0</v>
       </c>
-      <c r="Q5" s="15">
-        <v>0</v>
-      </c>
-      <c r="R5" s="18">
-        <v>0</v>
-      </c>
-      <c r="S5" s="18">
-        <v>0</v>
-      </c>
-      <c r="T5" s="18">
-        <v>0</v>
-      </c>
-      <c r="U5" s="18">
-        <v>0</v>
-      </c>
-      <c r="V5" s="18">
+      <c r="Q5">
+        <v>0</v>
+      </c>
+      <c r="R5">
+        <v>0</v>
+      </c>
+      <c r="S5">
+        <v>0</v>
+      </c>
+      <c r="T5">
+        <v>0</v>
+      </c>
+      <c r="U5">
+        <v>0</v>
+      </c>
+      <c r="V5">
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="B6" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -1576,7 +1532,7 @@
       <c r="D6">
         <v>0</v>
       </c>
-      <c r="E6" s="15">
+      <c r="E6">
         <v>0</v>
       </c>
       <c r="F6">
@@ -1612,39 +1568,39 @@
       <c r="P6">
         <v>0</v>
       </c>
-      <c r="Q6" s="15">
-        <v>0</v>
-      </c>
-      <c r="R6" s="18">
-        <v>0</v>
-      </c>
-      <c r="S6" s="18">
-        <v>0</v>
-      </c>
-      <c r="T6" s="18">
-        <v>0</v>
-      </c>
-      <c r="U6" s="18">
-        <v>0</v>
-      </c>
-      <c r="V6" s="18">
+      <c r="Q6">
+        <v>0</v>
+      </c>
+      <c r="R6">
+        <v>0</v>
+      </c>
+      <c r="S6">
+        <v>0</v>
+      </c>
+      <c r="T6">
+        <v>0</v>
+      </c>
+      <c r="U6">
+        <v>0</v>
+      </c>
+      <c r="V6">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="B7" t="s">
-        <v>22</v>
-      </c>
-      <c r="C7" s="5">
+        <v>33</v>
+      </c>
+      <c r="C7">
         <v>18451</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D7">
         <v>11632</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7">
         <v>1179</v>
       </c>
       <c r="F7">
@@ -1665,46 +1621,46 @@
       <c r="K7">
         <v>13</v>
       </c>
-      <c r="L7">
-        <v>-4.9292343460000003</v>
+      <c r="L7" s="1">
+        <v>-1.3281700000000001</v>
       </c>
       <c r="M7">
-        <v>1.0557509257487754</v>
+        <v>0.51413189636834655</v>
       </c>
       <c r="N7">
-        <v>21.626523017826401</v>
+        <v>50.24629209960564</v>
       </c>
       <c r="O7">
-        <v>-13.776858590186404</v>
+        <v>-44.875745348490668</v>
       </c>
       <c r="P7">
-        <v>-5.1727313299650071</v>
-      </c>
-      <c r="Q7" s="17">
+        <v>-0.73722366738806788</v>
+      </c>
+      <c r="Q7">
         <v>11.41</v>
       </c>
-      <c r="R7" s="19">
+      <c r="R7">
         <v>103.89</v>
       </c>
-      <c r="S7" s="20">
+      <c r="S7">
         <v>0.04</v>
       </c>
       <c r="T7">
-        <v>-0.27999999999999997</v>
-      </c>
-      <c r="U7" s="18">
+        <v>-0.28000000000000003</v>
+      </c>
+      <c r="U7">
         <v>0</v>
       </c>
       <c r="V7">
-        <v>-35.946843853820596</v>
+        <v>-35.94684385</v>
       </c>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="B8" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="C8">
         <v>0</v>
@@ -1712,7 +1668,7 @@
       <c r="D8">
         <v>0</v>
       </c>
-      <c r="E8" s="15">
+      <c r="E8">
         <v>0</v>
       </c>
       <c r="F8">
@@ -1748,31 +1704,31 @@
       <c r="P8">
         <v>0</v>
       </c>
-      <c r="Q8" s="15">
-        <v>0</v>
-      </c>
-      <c r="R8" s="18">
-        <v>0</v>
-      </c>
-      <c r="S8" s="18">
-        <v>0</v>
-      </c>
-      <c r="T8" s="18">
-        <v>0</v>
-      </c>
-      <c r="U8" s="18">
-        <v>0</v>
-      </c>
-      <c r="V8" s="18">
+      <c r="Q8">
+        <v>0</v>
+      </c>
+      <c r="R8">
+        <v>0</v>
+      </c>
+      <c r="S8">
+        <v>0</v>
+      </c>
+      <c r="T8">
+        <v>0</v>
+      </c>
+      <c r="U8">
+        <v>0</v>
+      </c>
+      <c r="V8">
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="B9" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="C9">
         <v>0</v>
@@ -1780,7 +1736,7 @@
       <c r="D9">
         <v>0</v>
       </c>
-      <c r="E9" s="15">
+      <c r="E9">
         <v>0</v>
       </c>
       <c r="F9">
@@ -1816,39 +1772,39 @@
       <c r="P9">
         <v>0</v>
       </c>
-      <c r="Q9" s="15">
-        <v>0</v>
-      </c>
-      <c r="R9" s="18">
-        <v>0</v>
-      </c>
-      <c r="S9" s="18">
-        <v>0</v>
-      </c>
-      <c r="T9" s="18">
-        <v>0</v>
-      </c>
-      <c r="U9" s="18">
-        <v>0</v>
-      </c>
-      <c r="V9" s="18">
+      <c r="Q9">
+        <v>0</v>
+      </c>
+      <c r="R9">
+        <v>0</v>
+      </c>
+      <c r="S9">
+        <v>0</v>
+      </c>
+      <c r="T9">
+        <v>0</v>
+      </c>
+      <c r="U9">
+        <v>0</v>
+      </c>
+      <c r="V9">
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="B10" t="s">
-        <v>28</v>
-      </c>
-      <c r="C10" s="8">
+        <v>39</v>
+      </c>
+      <c r="C10">
         <v>39181</v>
       </c>
-      <c r="D10" s="7">
+      <c r="D10">
         <v>31585</v>
       </c>
-      <c r="E10" s="6">
+      <c r="E10">
         <v>2867</v>
       </c>
       <c r="F10">
@@ -1869,46 +1825,46 @@
       <c r="K10">
         <v>14</v>
       </c>
-      <c r="L10">
-        <v>-4.8203515130000003</v>
+      <c r="L10" s="1">
+        <v>-2.6157300000000001</v>
       </c>
       <c r="M10">
-        <v>-0.31343854391289216</v>
+        <v>-0.11730382367723829</v>
       </c>
       <c r="N10">
-        <v>27.896518884511153</v>
+        <v>33.289055866441139</v>
       </c>
       <c r="O10">
-        <v>-15.144320140131102</v>
+        <v>13.745417707344279</v>
       </c>
       <c r="P10">
-        <v>-5.4503696277233082</v>
-      </c>
-      <c r="Q10" s="17">
+        <v>0.14176964862534397</v>
+      </c>
+      <c r="Q10">
         <v>10.199999999999999</v>
       </c>
-      <c r="R10" s="19">
+      <c r="R10">
         <v>95.41</v>
       </c>
-      <c r="S10" s="18">
+      <c r="S10">
         <v>-0.15</v>
       </c>
       <c r="T10">
-        <v>7.9999999999999988E-2</v>
-      </c>
-      <c r="U10" s="18">
-        <v>-65.550286084840735</v>
+        <v>0.08</v>
+      </c>
+      <c r="U10">
+        <v>-65.55</v>
       </c>
       <c r="V10">
-        <v>-37.291246100201867</v>
+        <v>-37.291246100000002</v>
       </c>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="B11" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="C11">
         <v>0</v>
@@ -1916,7 +1872,7 @@
       <c r="D11">
         <v>0</v>
       </c>
-      <c r="E11" s="15">
+      <c r="E11">
         <v>0</v>
       </c>
       <c r="F11">
@@ -1952,31 +1908,31 @@
       <c r="P11">
         <v>0</v>
       </c>
-      <c r="Q11" s="15">
-        <v>0</v>
-      </c>
-      <c r="R11" s="18">
-        <v>0</v>
-      </c>
-      <c r="S11" s="18">
-        <v>0</v>
-      </c>
-      <c r="T11" s="18">
-        <v>0</v>
-      </c>
-      <c r="U11" s="18">
-        <v>0</v>
-      </c>
-      <c r="V11" s="18">
+      <c r="Q11">
+        <v>0</v>
+      </c>
+      <c r="R11">
+        <v>0</v>
+      </c>
+      <c r="S11">
+        <v>0</v>
+      </c>
+      <c r="T11">
+        <v>0</v>
+      </c>
+      <c r="U11">
+        <v>0</v>
+      </c>
+      <c r="V11">
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="B12" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="C12">
         <v>0</v>
@@ -1984,7 +1940,7 @@
       <c r="D12">
         <v>0</v>
       </c>
-      <c r="E12" s="15">
+      <c r="E12">
         <v>0</v>
       </c>
       <c r="F12">
@@ -2020,31 +1976,31 @@
       <c r="P12">
         <v>0</v>
       </c>
-      <c r="Q12" s="15">
-        <v>0</v>
-      </c>
-      <c r="R12" s="18">
-        <v>0</v>
-      </c>
-      <c r="S12" s="18">
-        <v>0</v>
-      </c>
-      <c r="T12" s="18">
-        <v>0</v>
-      </c>
-      <c r="U12" s="18">
-        <v>0</v>
-      </c>
-      <c r="V12" s="18">
+      <c r="Q12">
+        <v>0</v>
+      </c>
+      <c r="R12">
+        <v>0</v>
+      </c>
+      <c r="S12">
+        <v>0</v>
+      </c>
+      <c r="T12">
+        <v>0</v>
+      </c>
+      <c r="U12">
+        <v>0</v>
+      </c>
+      <c r="V12">
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="B13" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="C13">
         <v>0</v>
@@ -2052,7 +2008,7 @@
       <c r="D13">
         <v>0</v>
       </c>
-      <c r="E13" s="15">
+      <c r="E13">
         <v>0</v>
       </c>
       <c r="F13">
@@ -2088,39 +2044,39 @@
       <c r="P13">
         <v>0</v>
       </c>
-      <c r="Q13" s="15">
-        <v>0</v>
-      </c>
-      <c r="R13" s="18">
-        <v>0</v>
-      </c>
-      <c r="S13" s="18">
-        <v>0</v>
-      </c>
-      <c r="T13" s="18">
-        <v>0</v>
-      </c>
-      <c r="U13" s="18">
-        <v>0</v>
-      </c>
-      <c r="V13" s="18">
+      <c r="Q13">
+        <v>0</v>
+      </c>
+      <c r="R13">
+        <v>0</v>
+      </c>
+      <c r="S13">
+        <v>0</v>
+      </c>
+      <c r="T13">
+        <v>0</v>
+      </c>
+      <c r="U13">
+        <v>0</v>
+      </c>
+      <c r="V13">
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>35</v>
+        <v>46</v>
       </c>
       <c r="B14" t="s">
-        <v>36</v>
-      </c>
-      <c r="C14" s="11">
+        <v>47</v>
+      </c>
+      <c r="C14">
         <v>57469</v>
       </c>
-      <c r="D14" s="12">
+      <c r="D14">
         <v>44171</v>
       </c>
-      <c r="E14" s="1">
+      <c r="E14">
         <v>1481</v>
       </c>
       <c r="F14">
@@ -2141,46 +2097,46 @@
       <c r="K14">
         <v>14</v>
       </c>
-      <c r="L14">
-        <v>-7.5196914540000002</v>
+      <c r="L14" s="1">
+        <v>-6.5356899999999998</v>
       </c>
       <c r="M14">
-        <v>0.16828363546258079</v>
-      </c>
-      <c r="N14">
-        <v>24.46372394497752</v>
+        <v>0.40868749733985255</v>
+      </c>
+      <c r="N14" s="2">
+        <v>53.869382743120099</v>
       </c>
       <c r="O14">
-        <v>-28.140992357099691</v>
+        <v>59.966007981339743</v>
       </c>
       <c r="P14">
-        <v>-11.384675542554627</v>
-      </c>
-      <c r="Q14" s="17">
+        <v>-3.9696697997767623</v>
+      </c>
+      <c r="Q14">
         <v>4.53</v>
       </c>
-      <c r="R14" s="19">
+      <c r="R14">
         <v>93.59</v>
       </c>
-      <c r="S14" s="20">
+      <c r="S14">
         <v>0.02</v>
       </c>
       <c r="T14">
         <v>-0.06</v>
       </c>
       <c r="U14">
-        <v>-66.488825953857457</v>
+        <v>-66.488825950000006</v>
       </c>
       <c r="V14">
-        <v>-37.738771295818275</v>
+        <v>-37.738771300000003</v>
       </c>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="B15" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="C15">
         <v>0</v>
@@ -2188,7 +2144,7 @@
       <c r="D15">
         <v>0</v>
       </c>
-      <c r="E15" s="15">
+      <c r="E15">
         <v>0</v>
       </c>
       <c r="F15">
@@ -2224,31 +2180,31 @@
       <c r="P15">
         <v>0</v>
       </c>
-      <c r="Q15" s="15">
-        <v>0</v>
-      </c>
-      <c r="R15" s="18">
-        <v>0</v>
-      </c>
-      <c r="S15" s="18">
-        <v>0</v>
-      </c>
-      <c r="T15" s="18">
-        <v>0</v>
-      </c>
-      <c r="U15" s="18">
-        <v>0</v>
-      </c>
-      <c r="V15" s="18">
+      <c r="Q15">
+        <v>0</v>
+      </c>
+      <c r="R15">
+        <v>0</v>
+      </c>
+      <c r="S15">
+        <v>0</v>
+      </c>
+      <c r="T15">
+        <v>0</v>
+      </c>
+      <c r="U15">
+        <v>0</v>
+      </c>
+      <c r="V15">
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="B16" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="C16">
         <v>0</v>
@@ -2256,7 +2212,7 @@
       <c r="D16">
         <v>0</v>
       </c>
-      <c r="E16" s="15">
+      <c r="E16">
         <v>0</v>
       </c>
       <c r="F16">
@@ -2292,31 +2248,31 @@
       <c r="P16">
         <v>0</v>
       </c>
-      <c r="Q16" s="15">
-        <v>0</v>
-      </c>
-      <c r="R16" s="18">
-        <v>0</v>
-      </c>
-      <c r="S16" s="18">
-        <v>0</v>
-      </c>
-      <c r="T16" s="18">
-        <v>0</v>
-      </c>
-      <c r="U16" s="18">
-        <v>0</v>
-      </c>
-      <c r="V16" s="18">
+      <c r="Q16">
+        <v>0</v>
+      </c>
+      <c r="R16">
+        <v>0</v>
+      </c>
+      <c r="S16">
+        <v>0</v>
+      </c>
+      <c r="T16">
+        <v>0</v>
+      </c>
+      <c r="U16">
+        <v>0</v>
+      </c>
+      <c r="V16">
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="B17" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="C17">
         <v>0</v>
@@ -2324,7 +2280,7 @@
       <c r="D17">
         <v>0</v>
       </c>
-      <c r="E17" s="15">
+      <c r="E17">
         <v>0</v>
       </c>
       <c r="F17">
@@ -2360,31 +2316,31 @@
       <c r="P17">
         <v>0</v>
       </c>
-      <c r="Q17" s="15">
-        <v>0</v>
-      </c>
-      <c r="R17" s="18">
-        <v>0</v>
-      </c>
-      <c r="S17" s="18">
-        <v>0</v>
-      </c>
-      <c r="T17" s="18">
-        <v>0</v>
-      </c>
-      <c r="U17" s="18">
-        <v>0</v>
-      </c>
-      <c r="V17" s="18">
+      <c r="Q17">
+        <v>0</v>
+      </c>
+      <c r="R17">
+        <v>0</v>
+      </c>
+      <c r="S17">
+        <v>0</v>
+      </c>
+      <c r="T17">
+        <v>0</v>
+      </c>
+      <c r="U17">
+        <v>0</v>
+      </c>
+      <c r="V17">
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>43</v>
+        <v>54</v>
       </c>
       <c r="B18" t="s">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="C18">
         <v>0</v>
@@ -2392,7 +2348,7 @@
       <c r="D18">
         <v>0</v>
       </c>
-      <c r="E18" s="15">
+      <c r="E18">
         <v>0</v>
       </c>
       <c r="F18">
@@ -2428,31 +2384,31 @@
       <c r="P18">
         <v>0</v>
       </c>
-      <c r="Q18" s="15">
-        <v>0</v>
-      </c>
-      <c r="R18" s="18">
-        <v>0</v>
-      </c>
-      <c r="S18" s="18">
-        <v>0</v>
-      </c>
-      <c r="T18" s="18">
-        <v>0</v>
-      </c>
-      <c r="U18" s="18">
-        <v>0</v>
-      </c>
-      <c r="V18" s="18">
+      <c r="Q18">
+        <v>0</v>
+      </c>
+      <c r="R18">
+        <v>0</v>
+      </c>
+      <c r="S18">
+        <v>0</v>
+      </c>
+      <c r="T18">
+        <v>0</v>
+      </c>
+      <c r="U18">
+        <v>0</v>
+      </c>
+      <c r="V18">
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="B19" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="C19">
         <v>0</v>
@@ -2460,7 +2416,7 @@
       <c r="D19">
         <v>0</v>
       </c>
-      <c r="E19" s="15">
+      <c r="E19">
         <v>0</v>
       </c>
       <c r="F19">
@@ -2496,31 +2452,31 @@
       <c r="P19">
         <v>0</v>
       </c>
-      <c r="Q19" s="15">
-        <v>0</v>
-      </c>
-      <c r="R19" s="18">
-        <v>0</v>
-      </c>
-      <c r="S19" s="18">
-        <v>0</v>
-      </c>
-      <c r="T19" s="18">
-        <v>0</v>
-      </c>
-      <c r="U19" s="18">
-        <v>0</v>
-      </c>
-      <c r="V19" s="18">
+      <c r="Q19">
+        <v>0</v>
+      </c>
+      <c r="R19">
+        <v>0</v>
+      </c>
+      <c r="S19">
+        <v>0</v>
+      </c>
+      <c r="T19">
+        <v>0</v>
+      </c>
+      <c r="U19">
+        <v>0</v>
+      </c>
+      <c r="V19">
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="B20" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="C20">
         <v>0</v>
@@ -2528,7 +2484,7 @@
       <c r="D20">
         <v>0</v>
       </c>
-      <c r="E20" s="15">
+      <c r="E20">
         <v>0</v>
       </c>
       <c r="F20">
@@ -2564,31 +2520,31 @@
       <c r="P20">
         <v>0</v>
       </c>
-      <c r="Q20" s="15">
-        <v>0</v>
-      </c>
-      <c r="R20" s="18">
-        <v>0</v>
-      </c>
-      <c r="S20" s="18">
-        <v>0</v>
-      </c>
-      <c r="T20" s="18">
-        <v>0</v>
-      </c>
-      <c r="U20" s="18">
-        <v>0</v>
-      </c>
-      <c r="V20" s="18">
+      <c r="Q20">
+        <v>0</v>
+      </c>
+      <c r="R20">
+        <v>0</v>
+      </c>
+      <c r="S20">
+        <v>0</v>
+      </c>
+      <c r="T20">
+        <v>0</v>
+      </c>
+      <c r="U20">
+        <v>0</v>
+      </c>
+      <c r="V20">
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>49</v>
+        <v>60</v>
       </c>
       <c r="B21" t="s">
-        <v>50</v>
+        <v>61</v>
       </c>
       <c r="C21">
         <v>0</v>
@@ -2596,7 +2552,7 @@
       <c r="D21">
         <v>0</v>
       </c>
-      <c r="E21" s="15">
+      <c r="E21">
         <v>0</v>
       </c>
       <c r="F21">
@@ -2632,31 +2588,31 @@
       <c r="P21">
         <v>0</v>
       </c>
-      <c r="Q21" s="15">
-        <v>0</v>
-      </c>
-      <c r="R21" s="18">
-        <v>0</v>
-      </c>
-      <c r="S21" s="18">
-        <v>0</v>
-      </c>
-      <c r="T21" s="18">
-        <v>0</v>
-      </c>
-      <c r="U21" s="18">
-        <v>0</v>
-      </c>
-      <c r="V21" s="18">
+      <c r="Q21">
+        <v>0</v>
+      </c>
+      <c r="R21">
+        <v>0</v>
+      </c>
+      <c r="S21">
+        <v>0</v>
+      </c>
+      <c r="T21">
+        <v>0</v>
+      </c>
+      <c r="U21">
+        <v>0</v>
+      </c>
+      <c r="V21">
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="B22" t="s">
-        <v>52</v>
+        <v>63</v>
       </c>
       <c r="C22">
         <v>0</v>
@@ -2664,7 +2620,7 @@
       <c r="D22">
         <v>0</v>
       </c>
-      <c r="E22" s="15">
+      <c r="E22">
         <v>0</v>
       </c>
       <c r="F22">
@@ -2700,31 +2656,31 @@
       <c r="P22">
         <v>0</v>
       </c>
-      <c r="Q22" s="15">
-        <v>0</v>
-      </c>
-      <c r="R22" s="18">
-        <v>0</v>
-      </c>
-      <c r="S22" s="18">
-        <v>0</v>
-      </c>
-      <c r="T22" s="18">
-        <v>0</v>
-      </c>
-      <c r="U22" s="18">
-        <v>0</v>
-      </c>
-      <c r="V22" s="18">
+      <c r="Q22">
+        <v>0</v>
+      </c>
+      <c r="R22">
+        <v>0</v>
+      </c>
+      <c r="S22">
+        <v>0</v>
+      </c>
+      <c r="T22">
+        <v>0</v>
+      </c>
+      <c r="U22">
+        <v>0</v>
+      </c>
+      <c r="V22">
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>53</v>
+        <v>64</v>
       </c>
       <c r="B23" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="C23">
         <v>0</v>
@@ -2732,7 +2688,7 @@
       <c r="D23">
         <v>0</v>
       </c>
-      <c r="E23" s="15">
+      <c r="E23">
         <v>0</v>
       </c>
       <c r="F23">
@@ -2768,31 +2724,31 @@
       <c r="P23">
         <v>0</v>
       </c>
-      <c r="Q23" s="15">
-        <v>0</v>
-      </c>
-      <c r="R23" s="18">
-        <v>0</v>
-      </c>
-      <c r="S23" s="18">
-        <v>0</v>
-      </c>
-      <c r="T23" s="18">
-        <v>0</v>
-      </c>
-      <c r="U23" s="18">
-        <v>0</v>
-      </c>
-      <c r="V23" s="18">
+      <c r="Q23">
+        <v>0</v>
+      </c>
+      <c r="R23">
+        <v>0</v>
+      </c>
+      <c r="S23">
+        <v>0</v>
+      </c>
+      <c r="T23">
+        <v>0</v>
+      </c>
+      <c r="U23">
+        <v>0</v>
+      </c>
+      <c r="V23">
         <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="B24" t="s">
-        <v>56</v>
+        <v>67</v>
       </c>
       <c r="C24">
         <v>0</v>
@@ -2800,7 +2756,7 @@
       <c r="D24">
         <v>0</v>
       </c>
-      <c r="E24" s="15">
+      <c r="E24">
         <v>0</v>
       </c>
       <c r="F24">
@@ -2836,31 +2792,31 @@
       <c r="P24">
         <v>0</v>
       </c>
-      <c r="Q24" s="15">
-        <v>0</v>
-      </c>
-      <c r="R24" s="18">
-        <v>0</v>
-      </c>
-      <c r="S24" s="18">
-        <v>0</v>
-      </c>
-      <c r="T24" s="18">
-        <v>0</v>
-      </c>
-      <c r="U24" s="18">
-        <v>0</v>
-      </c>
-      <c r="V24" s="18">
+      <c r="Q24">
+        <v>0</v>
+      </c>
+      <c r="R24">
+        <v>0</v>
+      </c>
+      <c r="S24">
+        <v>0</v>
+      </c>
+      <c r="T24">
+        <v>0</v>
+      </c>
+      <c r="U24">
+        <v>0</v>
+      </c>
+      <c r="V24">
         <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>57</v>
+        <v>68</v>
       </c>
       <c r="B25" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
       <c r="C25">
         <v>0</v>
@@ -2868,7 +2824,7 @@
       <c r="D25">
         <v>0</v>
       </c>
-      <c r="E25" s="15">
+      <c r="E25">
         <v>0</v>
       </c>
       <c r="F25">
@@ -2904,31 +2860,31 @@
       <c r="P25">
         <v>0</v>
       </c>
-      <c r="Q25" s="15">
-        <v>0</v>
-      </c>
-      <c r="R25" s="18">
-        <v>0</v>
-      </c>
-      <c r="S25" s="18">
-        <v>0</v>
-      </c>
-      <c r="T25" s="18">
-        <v>0</v>
-      </c>
-      <c r="U25" s="18">
-        <v>0</v>
-      </c>
-      <c r="V25" s="18">
+      <c r="Q25">
+        <v>0</v>
+      </c>
+      <c r="R25">
+        <v>0</v>
+      </c>
+      <c r="S25">
+        <v>0</v>
+      </c>
+      <c r="T25">
+        <v>0</v>
+      </c>
+      <c r="U25">
+        <v>0</v>
+      </c>
+      <c r="V25">
         <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
       <c r="B26" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="C26">
         <v>0</v>
@@ -2936,7 +2892,7 @@
       <c r="D26">
         <v>0</v>
       </c>
-      <c r="E26" s="15">
+      <c r="E26">
         <v>0</v>
       </c>
       <c r="F26">
@@ -2972,39 +2928,39 @@
       <c r="P26">
         <v>0</v>
       </c>
-      <c r="Q26" s="15">
-        <v>0</v>
-      </c>
-      <c r="R26" s="18">
-        <v>0</v>
-      </c>
-      <c r="S26" s="18">
-        <v>0</v>
-      </c>
-      <c r="T26" s="18">
-        <v>0</v>
-      </c>
-      <c r="U26" s="18">
-        <v>0</v>
-      </c>
-      <c r="V26" s="18">
+      <c r="Q26">
+        <v>0</v>
+      </c>
+      <c r="R26">
+        <v>0</v>
+      </c>
+      <c r="S26">
+        <v>0</v>
+      </c>
+      <c r="T26">
+        <v>0</v>
+      </c>
+      <c r="U26">
+        <v>0</v>
+      </c>
+      <c r="V26">
         <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>61</v>
+        <v>72</v>
       </c>
       <c r="B27" t="s">
-        <v>62</v>
-      </c>
-      <c r="C27" s="13">
+        <v>73</v>
+      </c>
+      <c r="C27">
         <v>13747</v>
       </c>
-      <c r="D27" s="16">
+      <c r="D27">
         <v>10345</v>
       </c>
-      <c r="E27" s="14">
+      <c r="E27">
         <v>386</v>
       </c>
       <c r="F27">
@@ -3025,46 +2981,46 @@
       <c r="K27">
         <v>12</v>
       </c>
-      <c r="L27">
-        <v>-6.1813050379999996</v>
+      <c r="L27" s="1">
+        <v>-3.2630599999999998</v>
       </c>
       <c r="M27">
-        <v>8.0933606468208161</v>
+        <v>8.6718011302252176</v>
       </c>
       <c r="N27">
-        <v>46.232635762743755</v>
+        <v>41.731840382997888</v>
       </c>
       <c r="O27">
-        <v>122.25709618019836</v>
+        <v>340.601002457427</v>
       </c>
       <c r="P27">
-        <v>-0.41498546380446105</v>
-      </c>
-      <c r="Q27" s="17">
+        <v>7.7334573954840318</v>
+      </c>
+      <c r="Q27">
         <v>8.7200000000000006</v>
       </c>
-      <c r="R27" s="18">
+      <c r="R27">
         <v>101.81</v>
       </c>
-      <c r="S27" s="20">
+      <c r="S27">
         <v>0.02</v>
       </c>
       <c r="T27">
-        <v>-0.16999999999999998</v>
+        <v>-0.17</v>
       </c>
       <c r="U27">
-        <v>-54.007451575054375</v>
+        <v>-54.007451580000001</v>
       </c>
       <c r="V27">
-        <v>-5.6249999999999982</v>
+        <v>-5.625</v>
       </c>
     </row>
     <row r="28" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>63</v>
+        <v>74</v>
       </c>
       <c r="B28" t="s">
-        <v>64</v>
+        <v>75</v>
       </c>
       <c r="C28">
         <v>0</v>
@@ -3072,7 +3028,7 @@
       <c r="D28">
         <v>0</v>
       </c>
-      <c r="E28" s="15">
+      <c r="E28">
         <v>0</v>
       </c>
       <c r="F28">
@@ -3108,31 +3064,31 @@
       <c r="P28">
         <v>0</v>
       </c>
-      <c r="Q28" s="15">
-        <v>0</v>
-      </c>
-      <c r="R28" s="18">
-        <v>0</v>
-      </c>
-      <c r="S28" s="18">
-        <v>0</v>
-      </c>
-      <c r="T28" s="18">
-        <v>0</v>
-      </c>
-      <c r="U28" s="18">
-        <v>0</v>
-      </c>
-      <c r="V28" s="18">
+      <c r="Q28">
+        <v>0</v>
+      </c>
+      <c r="R28">
+        <v>0</v>
+      </c>
+      <c r="S28">
+        <v>0</v>
+      </c>
+      <c r="T28">
+        <v>0</v>
+      </c>
+      <c r="U28">
+        <v>0</v>
+      </c>
+      <c r="V28">
         <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>65</v>
+        <v>76</v>
       </c>
       <c r="B29" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="C29">
         <v>0</v>
@@ -3140,7 +3096,7 @@
       <c r="D29">
         <v>0</v>
       </c>
-      <c r="E29" s="15">
+      <c r="E29">
         <v>0</v>
       </c>
       <c r="F29">
@@ -3176,39 +3132,39 @@
       <c r="P29">
         <v>0</v>
       </c>
-      <c r="Q29" s="15">
-        <v>0</v>
-      </c>
-      <c r="R29" s="18">
-        <v>0</v>
-      </c>
-      <c r="S29" s="18">
-        <v>0</v>
-      </c>
-      <c r="T29" s="18">
-        <v>0</v>
-      </c>
-      <c r="U29" s="18">
-        <v>0</v>
-      </c>
-      <c r="V29" s="18">
+      <c r="Q29">
+        <v>0</v>
+      </c>
+      <c r="R29">
+        <v>0</v>
+      </c>
+      <c r="S29">
+        <v>0</v>
+      </c>
+      <c r="T29">
+        <v>0</v>
+      </c>
+      <c r="U29">
+        <v>0</v>
+      </c>
+      <c r="V29">
         <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>67</v>
+        <v>78</v>
       </c>
       <c r="B30" t="s">
-        <v>68</v>
-      </c>
-      <c r="C30" s="9">
+        <v>79</v>
+      </c>
+      <c r="C30">
         <v>15231</v>
       </c>
-      <c r="D30" s="10">
+      <c r="D30">
         <v>8319</v>
       </c>
-      <c r="E30" s="2">
+      <c r="E30">
         <v>306</v>
       </c>
       <c r="F30">
@@ -3229,46 +3185,46 @@
       <c r="K30">
         <v>13</v>
       </c>
-      <c r="L30">
-        <v>-6.3433217040000001</v>
+      <c r="L30" s="1">
+        <v>-2.75705</v>
       </c>
       <c r="M30">
-        <v>-0.46427124120495356</v>
+        <v>-5.3865459600981547</v>
       </c>
       <c r="N30">
-        <v>65.165477987395477</v>
+        <v>70.191491344294448</v>
       </c>
       <c r="O30">
-        <v>-10.154540478150164</v>
+        <v>32.640851527260864</v>
       </c>
       <c r="P30">
-        <v>-4.9507099043534319</v>
-      </c>
-      <c r="Q30" s="17">
+        <v>-1.7433818172850866</v>
+      </c>
+      <c r="Q30">
         <v>7.88</v>
       </c>
-      <c r="R30" s="19">
+      <c r="R30">
         <v>101.35</v>
       </c>
-      <c r="S30" s="20">
+      <c r="S30">
         <v>-0.01</v>
       </c>
       <c r="T30">
         <v>0.25</v>
       </c>
-      <c r="U30" s="18">
+      <c r="U30">
         <v>0</v>
       </c>
       <c r="V30">
-        <v>-17.668414683340053</v>
+        <v>-17.668414680000001</v>
       </c>
     </row>
     <row r="31" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>69</v>
+        <v>80</v>
       </c>
       <c r="B31" t="s">
-        <v>70</v>
+        <v>81</v>
       </c>
       <c r="C31">
         <v>0</v>
@@ -3276,7 +3232,7 @@
       <c r="D31">
         <v>0</v>
       </c>
-      <c r="E31" s="15">
+      <c r="E31">
         <v>0</v>
       </c>
       <c r="F31">
@@ -3312,31 +3268,31 @@
       <c r="P31">
         <v>0</v>
       </c>
-      <c r="Q31" s="15">
-        <v>0</v>
-      </c>
-      <c r="R31" s="18">
-        <v>0</v>
-      </c>
-      <c r="S31" s="18">
-        <v>0</v>
-      </c>
-      <c r="T31" s="18">
-        <v>0</v>
-      </c>
-      <c r="U31" s="18">
-        <v>0</v>
-      </c>
-      <c r="V31" s="18">
+      <c r="Q31">
+        <v>0</v>
+      </c>
+      <c r="R31">
+        <v>0</v>
+      </c>
+      <c r="S31">
+        <v>0</v>
+      </c>
+      <c r="T31">
+        <v>0</v>
+      </c>
+      <c r="U31">
+        <v>0</v>
+      </c>
+      <c r="V31">
         <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>71</v>
+        <v>82</v>
       </c>
       <c r="B32" t="s">
-        <v>72</v>
+        <v>83</v>
       </c>
       <c r="C32">
         <v>0</v>
@@ -3344,7 +3300,7 @@
       <c r="D32">
         <v>0</v>
       </c>
-      <c r="E32" s="15">
+      <c r="E32">
         <v>0</v>
       </c>
       <c r="F32">
@@ -3380,31 +3336,31 @@
       <c r="P32">
         <v>0</v>
       </c>
-      <c r="Q32" s="15">
-        <v>0</v>
-      </c>
-      <c r="R32" s="18">
-        <v>0</v>
-      </c>
-      <c r="S32" s="18">
-        <v>0</v>
-      </c>
-      <c r="T32" s="18">
-        <v>0</v>
-      </c>
-      <c r="U32" s="18">
-        <v>0</v>
-      </c>
-      <c r="V32" s="18">
+      <c r="Q32">
+        <v>0</v>
+      </c>
+      <c r="R32">
+        <v>0</v>
+      </c>
+      <c r="S32">
+        <v>0</v>
+      </c>
+      <c r="T32">
+        <v>0</v>
+      </c>
+      <c r="U32">
+        <v>0</v>
+      </c>
+      <c r="V32">
         <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>73</v>
+        <v>84</v>
       </c>
       <c r="B33" t="s">
-        <v>74</v>
+        <v>85</v>
       </c>
       <c r="C33">
         <v>0</v>
@@ -3412,7 +3368,7 @@
       <c r="D33">
         <v>0</v>
       </c>
-      <c r="E33" s="15">
+      <c r="E33">
         <v>0</v>
       </c>
       <c r="F33">
@@ -3448,31 +3404,31 @@
       <c r="P33">
         <v>0</v>
       </c>
-      <c r="Q33" s="15">
-        <v>0</v>
-      </c>
-      <c r="R33" s="18">
-        <v>0</v>
-      </c>
-      <c r="S33" s="18">
-        <v>0</v>
-      </c>
-      <c r="T33" s="18">
-        <v>0</v>
-      </c>
-      <c r="U33" s="18">
-        <v>0</v>
-      </c>
-      <c r="V33" s="18">
+      <c r="Q33">
+        <v>0</v>
+      </c>
+      <c r="R33">
+        <v>0</v>
+      </c>
+      <c r="S33">
+        <v>0</v>
+      </c>
+      <c r="T33">
+        <v>0</v>
+      </c>
+      <c r="U33">
+        <v>0</v>
+      </c>
+      <c r="V33">
         <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="B34" t="s">
-        <v>76</v>
+        <v>87</v>
       </c>
       <c r="C34">
         <v>0</v>
@@ -3480,7 +3436,7 @@
       <c r="D34">
         <v>0</v>
       </c>
-      <c r="E34" s="15">
+      <c r="E34">
         <v>0</v>
       </c>
       <c r="F34">
@@ -3516,31 +3472,31 @@
       <c r="P34">
         <v>0</v>
       </c>
-      <c r="Q34" s="15">
-        <v>0</v>
-      </c>
-      <c r="R34" s="18">
-        <v>0</v>
-      </c>
-      <c r="S34" s="18">
-        <v>0</v>
-      </c>
-      <c r="T34" s="18">
-        <v>0</v>
-      </c>
-      <c r="U34" s="18">
-        <v>0</v>
-      </c>
-      <c r="V34" s="18">
+      <c r="Q34">
+        <v>0</v>
+      </c>
+      <c r="R34">
+        <v>0</v>
+      </c>
+      <c r="S34">
+        <v>0</v>
+      </c>
+      <c r="T34">
+        <v>0</v>
+      </c>
+      <c r="U34">
+        <v>0</v>
+      </c>
+      <c r="V34">
         <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>77</v>
+        <v>88</v>
       </c>
       <c r="B35" t="s">
-        <v>78</v>
+        <v>89</v>
       </c>
       <c r="C35">
         <v>0</v>
@@ -3548,7 +3504,7 @@
       <c r="D35">
         <v>0</v>
       </c>
-      <c r="E35" s="15">
+      <c r="E35">
         <v>0</v>
       </c>
       <c r="F35">
@@ -3584,28 +3540,24 @@
       <c r="P35">
         <v>0</v>
       </c>
-      <c r="Q35" s="15">
-        <v>0</v>
-      </c>
-      <c r="R35" s="18">
-        <v>0</v>
-      </c>
-      <c r="S35" s="18">
-        <v>0</v>
-      </c>
-      <c r="T35" s="18">
-        <v>0</v>
-      </c>
-      <c r="U35" s="18">
-        <v>0</v>
-      </c>
-      <c r="V35" s="18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="S36" s="18"/>
-      <c r="T36" s="18"/>
+      <c r="Q35">
+        <v>0</v>
+      </c>
+      <c r="R35">
+        <v>0</v>
+      </c>
+      <c r="S35">
+        <v>0</v>
+      </c>
+      <c r="T35">
+        <v>0</v>
+      </c>
+      <c r="U35">
+        <v>0</v>
+      </c>
+      <c r="V35">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
updated temporal_data for Indonesia to include mobility data through mid-September
</commit_message>
<xml_diff>
--- a/Data/Indonesia/Misc/ShapefileAddingIndonesia.xlsx
+++ b/Data/Indonesia/Misc/ShapefileAddingIndonesia.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20367"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20368"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\slomb\OneDrive\Desktop\Vida_Modeling\Data\Indonesia\Misc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{B00A4836-DDB3-40AA-B597-0123B4A33EE0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30B4BEAC-52B9-43F8-B305-FF269FA83F0F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="16725"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12810" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ShapefileAddingIndonesia" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
@@ -295,7 +295,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1155,19 +1155,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+      <selection activeCell="A31" sqref="A31:E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="6.140625" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="10.42578125" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="6.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7.85546875" bestFit="1" customWidth="1"/>

</xml_diff>